<commit_message>
£BME FY16, 17, 18, 19 data entry
</commit_message>
<xml_diff>
--- a/£BME.xlsx
+++ b/£BME.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{375092EB-F279-495C-858B-3096B70283A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29CFECD-F4CC-4B99-A485-E480B9A4C740}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" activeTab="1" xr2:uid="{0B0D3E06-E58D-4F1F-A8B8-3BC216B2A3D5}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="135">
   <si>
     <t>£BME</t>
   </si>
@@ -456,6 +456,15 @@
   </si>
   <si>
     <t>(EST.)</t>
+  </si>
+  <si>
+    <t>B&amp;M Sells entire German Business Jawoll for 12.5m Euro after 'disappointing' financial performance</t>
+  </si>
+  <si>
+    <t>Jawoll</t>
+  </si>
+  <si>
+    <t>Germany</t>
   </si>
 </sst>
 </file>
@@ -724,7 +733,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -886,6 +895,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -980,7 +990,7 @@
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1030,7 +1040,7 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>115</xdr:row>
+      <xdr:row>117</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1373,7 +1383,7 @@
   <dimension ref="B2:X40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C36" sqref="C36:D36"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1525,7 +1535,7 @@
         <v>6</v>
       </c>
       <c r="C9" s="22">
-        <f>+'Financial Model'!V86</f>
+        <f>+'Financial Model'!V88</f>
         <v>238</v>
       </c>
       <c r="D9" s="24" t="str">
@@ -1556,7 +1566,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="22">
-        <f>+'Financial Model'!V87</f>
+        <f>+'Financial Model'!V89</f>
         <v>954</v>
       </c>
       <c r="D10" s="24" t="str">
@@ -1726,8 +1736,12 @@
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="17"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="9"/>
+      <c r="F18" s="59">
+        <v>43891</v>
+      </c>
+      <c r="G18" s="91" t="s">
+        <v>132</v>
+      </c>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
@@ -1918,7 +1932,7 @@
         <v>19</v>
       </c>
       <c r="C28" s="51">
-        <f>+'Financial Model'!V61</f>
+        <f>+'Financial Model'!V63</f>
         <v>764</v>
       </c>
       <c r="D28" s="17"/>
@@ -2048,7 +2062,7 @@
         <v>31</v>
       </c>
       <c r="C35" s="45">
-        <f>C6/'Financial Model'!V84</f>
+        <f>C6/'Financial Model'!V86</f>
         <v>7.9778273551388885</v>
       </c>
       <c r="D35" s="46"/>
@@ -2202,22 +2216,23 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C31:D31" r:id="rId1" display="Link" xr:uid="{9BE3B3D4-9498-4B97-998C-C0C12FA77148}"/>
+    <hyperlink ref="G18" r:id="rId2" xr:uid="{87BBEC1A-B702-4F90-99BE-E634A1207125}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="125" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup paperSize="125" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E38EA70-0C15-460C-B41E-267C906FFAC5}">
-  <dimension ref="B1:AE105"/>
+  <dimension ref="B1:AE107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C64" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T22" sqref="T22"/>
+      <selection pane="bottomRight" activeCell="O92" sqref="O92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2248,13 +2263,13 @@
       <c r="O1" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="P1" s="30" t="s">
+      <c r="P1" s="31" t="s">
         <v>72</v>
       </c>
       <c r="Q1" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="R1" s="30" t="s">
+      <c r="R1" s="31" t="s">
         <v>70</v>
       </c>
       <c r="S1" s="30" t="s">
@@ -2304,6 +2319,18 @@
       <c r="H2" s="65"/>
       <c r="J2" s="65"/>
       <c r="L2" s="65"/>
+      <c r="O2" s="36">
+        <v>42455</v>
+      </c>
+      <c r="P2" s="36">
+        <v>42819</v>
+      </c>
+      <c r="Q2" s="36">
+        <v>43190</v>
+      </c>
+      <c r="R2" s="36">
+        <v>43554</v>
+      </c>
       <c r="S2" s="36">
         <v>43918</v>
       </c>
@@ -2327,6 +2354,12 @@
       <c r="H3" s="65"/>
       <c r="J3" s="65"/>
       <c r="L3" s="65"/>
+      <c r="P3" s="44">
+        <v>45071</v>
+      </c>
+      <c r="R3" s="44">
+        <v>45069</v>
+      </c>
       <c r="T3" s="44">
         <v>45080</v>
       </c>
@@ -2348,10 +2381,18 @@
       <c r="H4" s="66"/>
       <c r="J4" s="66"/>
       <c r="L4" s="66"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
+      <c r="O4" s="32">
+        <v>2035.2850000000001</v>
+      </c>
+      <c r="P4" s="32">
+        <v>2430.66</v>
+      </c>
+      <c r="Q4" s="32">
+        <v>3029.8020000000001</v>
+      </c>
+      <c r="R4" s="32">
+        <v>3486.2950000000001</v>
+      </c>
       <c r="S4" s="32">
         <v>3813.3870000000002</v>
       </c>
@@ -2373,10 +2414,18 @@
       <c r="B5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
+      <c r="O5" s="33">
+        <v>1332.2629999999999</v>
+      </c>
+      <c r="P5" s="33">
+        <v>1586.3240000000001</v>
+      </c>
+      <c r="Q5" s="33">
+        <v>2000.9269999999999</v>
+      </c>
+      <c r="R5" s="33">
+        <v>2296.681</v>
+      </c>
       <c r="S5" s="33">
         <v>2530.5790000000002</v>
       </c>
@@ -2405,19 +2454,19 @@
       <c r="L6" s="66"/>
       <c r="O6" s="32">
         <f t="shared" ref="O6" si="0">O4-O5</f>
-        <v>0</v>
+        <v>703.02200000000016</v>
       </c>
       <c r="P6" s="32">
         <f t="shared" ref="P6" si="1">P4-P5</f>
-        <v>0</v>
+        <v>844.33599999999979</v>
       </c>
       <c r="Q6" s="32">
         <f t="shared" ref="Q6" si="2">Q4-Q5</f>
-        <v>0</v>
+        <v>1028.8750000000002</v>
       </c>
       <c r="R6" s="32">
         <f t="shared" ref="R6" si="3">R4-R5</f>
-        <v>0</v>
+        <v>1189.614</v>
       </c>
       <c r="S6" s="32">
         <f t="shared" ref="S6" si="4">S4-S5</f>
@@ -2444,10 +2493,18 @@
       <c r="B7" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
+      <c r="O7" s="33">
+        <v>528.53</v>
+      </c>
+      <c r="P7" s="33">
+        <v>639.83299999999997</v>
+      </c>
+      <c r="Q7" s="33">
+        <v>789.072</v>
+      </c>
+      <c r="R7" s="33">
+        <v>925.05799999999999</v>
+      </c>
       <c r="S7" s="33">
         <f>966.928-16.932</f>
         <v>949.99599999999998</v>
@@ -2474,19 +2531,19 @@
       <c r="L8" s="66"/>
       <c r="O8" s="32">
         <f t="shared" ref="O8:T8" si="6">O6-O7</f>
-        <v>0</v>
+        <v>174.49200000000019</v>
       </c>
       <c r="P8" s="32">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>204.50299999999982</v>
       </c>
       <c r="Q8" s="32">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>239.80300000000022</v>
       </c>
       <c r="R8" s="32">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>264.55600000000004</v>
       </c>
       <c r="S8" s="32">
         <f t="shared" si="6"/>
@@ -2510,10 +2567,18 @@
       <c r="B9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="33"/>
+      <c r="O9" s="33">
+        <v>1.1659999999999999</v>
+      </c>
+      <c r="P9" s="33">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="Q9" s="33">
+        <v>1.7110000000000001</v>
+      </c>
+      <c r="R9" s="33">
+        <v>0.77500000000000002</v>
+      </c>
       <c r="S9" s="33">
         <v>0.879</v>
       </c>
@@ -2534,19 +2599,19 @@
       </c>
       <c r="O10" s="33">
         <f t="shared" ref="O10:T10" si="7">O8+O9</f>
-        <v>0</v>
+        <v>175.65800000000019</v>
       </c>
       <c r="P10" s="33">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>205.50799999999981</v>
       </c>
       <c r="Q10" s="33">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>241.51400000000024</v>
       </c>
       <c r="R10" s="33">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>265.33100000000002</v>
       </c>
       <c r="S10" s="33">
         <f t="shared" si="7"/>
@@ -2570,10 +2635,18 @@
       <c r="B11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O11" s="33"/>
-      <c r="P11" s="33"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="33"/>
+      <c r="O11" s="33">
+        <v>21.573</v>
+      </c>
+      <c r="P11" s="33">
+        <v>24.11</v>
+      </c>
+      <c r="Q11" s="33">
+        <v>23.948</v>
+      </c>
+      <c r="R11" s="33">
+        <v>25.951000000000001</v>
+      </c>
       <c r="S11" s="33">
         <v>57.206000000000003</v>
       </c>
@@ -2592,10 +2665,18 @@
       <c r="B12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="O12" s="33"/>
-      <c r="P12" s="33"/>
-      <c r="Q12" s="33"/>
-      <c r="R12" s="33"/>
+      <c r="O12" s="33">
+        <v>0.46</v>
+      </c>
+      <c r="P12" s="33">
+        <v>1.52</v>
+      </c>
+      <c r="Q12" s="33">
+        <v>0.182</v>
+      </c>
+      <c r="R12" s="33">
+        <v>0.36899999999999999</v>
+      </c>
       <c r="S12" s="33">
         <v>24.809000000000001</v>
       </c>
@@ -2614,10 +2695,18 @@
       <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="33"/>
-      <c r="R13" s="33"/>
+      <c r="O13" s="33">
+        <v>0</v>
+      </c>
+      <c r="P13" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="33">
+        <v>11.568</v>
+      </c>
+      <c r="R13" s="33">
+        <v>9.8569999999999993</v>
+      </c>
       <c r="S13" s="33">
         <f>0.213+0.134</f>
         <v>0.34699999999999998</v>
@@ -2639,19 +2728,19 @@
       </c>
       <c r="O14" s="33">
         <f t="shared" ref="O14:T14" si="8">O10-O11-O12+O13</f>
-        <v>0</v>
+        <v>153.62500000000017</v>
       </c>
       <c r="P14" s="33">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>179.87799999999979</v>
       </c>
       <c r="Q14" s="33">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>228.95200000000025</v>
       </c>
       <c r="R14" s="33">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>248.86800000000002</v>
       </c>
       <c r="S14" s="33">
         <f t="shared" si="8"/>
@@ -2675,10 +2764,18 @@
       <c r="B15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="O15" s="33"/>
-      <c r="P15" s="33"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="33"/>
+      <c r="O15" s="33">
+        <v>28.745000000000001</v>
+      </c>
+      <c r="P15" s="33">
+        <v>38.884999999999998</v>
+      </c>
+      <c r="Q15" s="33">
+        <v>43.511000000000003</v>
+      </c>
+      <c r="R15" s="33">
+        <v>46.716999999999999</v>
+      </c>
       <c r="S15" s="33">
         <v>57.246000000000002</v>
       </c>
@@ -2704,19 +2801,19 @@
       <c r="L16" s="66"/>
       <c r="O16" s="32">
         <f t="shared" ref="O16:T16" si="9">O14-O15</f>
-        <v>0</v>
+        <v>124.88000000000017</v>
       </c>
       <c r="P16" s="32">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>140.9929999999998</v>
       </c>
       <c r="Q16" s="32">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>185.44100000000026</v>
       </c>
       <c r="R16" s="32">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>202.15100000000001</v>
       </c>
       <c r="S16" s="32">
         <f t="shared" si="9"/>
@@ -2740,10 +2837,18 @@
       <c r="B17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O17" s="33"/>
-      <c r="P17" s="33"/>
-      <c r="Q17" s="33"/>
-      <c r="R17" s="33"/>
+      <c r="O17" s="33">
+        <v>5.5</v>
+      </c>
+      <c r="P17" s="33">
+        <v>7.4790000000000001</v>
+      </c>
+      <c r="Q17" s="33">
+        <v>-15.659000000000001</v>
+      </c>
+      <c r="R17" s="33">
+        <v>-2.2850000000000001</v>
+      </c>
       <c r="S17" s="33">
         <v>1.661</v>
       </c>
@@ -2762,10 +2867,18 @@
       <c r="B18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="O18" s="33"/>
-      <c r="P18" s="33"/>
-      <c r="Q18" s="33"/>
-      <c r="R18" s="33"/>
+      <c r="O18" s="33">
+        <v>0</v>
+      </c>
+      <c r="P18" s="33">
+        <v>-1.667</v>
+      </c>
+      <c r="Q18" s="33">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="R18" s="33">
+        <v>19.995999999999999</v>
+      </c>
       <c r="S18" s="33">
         <v>8.6790000000000003</v>
       </c>
@@ -2784,10 +2897,21 @@
       <c r="B19" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O19" s="33"/>
-      <c r="P19" s="33"/>
-      <c r="Q19" s="33"/>
-      <c r="R19" s="33"/>
+      <c r="O19" s="33">
+        <f>0.005+0.013</f>
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="P19" s="33">
+        <f>0.016+0.324</f>
+        <v>0.34</v>
+      </c>
+      <c r="Q19" s="33">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="R19" s="33">
+        <f>0.005-3.481</f>
+        <v>-3.476</v>
+      </c>
       <c r="S19" s="33">
         <v>-1.383</v>
       </c>
@@ -2813,19 +2937,19 @@
       <c r="L20" s="66"/>
       <c r="O20" s="32">
         <f t="shared" ref="O20:T20" si="10">O16+SUM(O17:O19)</f>
-        <v>0</v>
+        <v>130.39800000000017</v>
       </c>
       <c r="P20" s="32">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>147.14499999999978</v>
       </c>
       <c r="Q20" s="32">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>172.27300000000025</v>
       </c>
       <c r="R20" s="32">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>216.38600000000002</v>
       </c>
       <c r="S20" s="32">
         <f t="shared" si="10"/>
@@ -2854,12 +2978,28 @@
       <c r="H21" s="68"/>
       <c r="J21" s="68"/>
       <c r="L21" s="68"/>
+      <c r="O21" s="40">
+        <f t="shared" ref="O21" si="11">O20/O22</f>
+        <v>0.13033609035708055</v>
+      </c>
+      <c r="P21" s="40">
+        <f t="shared" ref="P21" si="12">P20/P22</f>
+        <v>0.14712322576258691</v>
+      </c>
+      <c r="Q21" s="40">
+        <f t="shared" ref="Q21" si="13">Q20/Q22</f>
+        <v>0.1721609232389717</v>
+      </c>
+      <c r="R21" s="40">
+        <f t="shared" ref="R21" si="14">R20/R22</f>
+        <v>0.21616680685784617</v>
+      </c>
       <c r="S21" s="40">
-        <f t="shared" ref="S21:T21" si="11">S20/S22</f>
+        <f t="shared" ref="S21:T21" si="15">S20/S22</f>
         <v>0.20361793777546799</v>
       </c>
       <c r="T21" s="40">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0.4101669339808835</v>
       </c>
       <c r="U21" s="40">
@@ -2867,7 +3007,7 @@
         <v>0.4355378942941539</v>
       </c>
       <c r="V21" s="40">
-        <f t="shared" ref="V21" si="12">V20/V22</f>
+        <f t="shared" ref="V21" si="16">V20/V22</f>
         <v>0.3853860799746005</v>
       </c>
       <c r="W21" s="81"/>
@@ -2881,6 +3021,18 @@
       <c r="H22" s="69"/>
       <c r="J22" s="69"/>
       <c r="L22" s="69"/>
+      <c r="O22" s="41">
+        <v>1000.475</v>
+      </c>
+      <c r="P22" s="41">
+        <v>1000.148</v>
+      </c>
+      <c r="Q22" s="41">
+        <v>1000.651</v>
+      </c>
+      <c r="R22" s="41">
+        <v>1001.014</v>
+      </c>
       <c r="S22" s="41">
         <v>1000.57</v>
       </c>
@@ -2907,6 +3059,25 @@
       <c r="H24" s="66"/>
       <c r="J24" s="66"/>
       <c r="L24" s="66"/>
+      <c r="O24" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="P24" s="38">
+        <f t="shared" ref="P24:T24" si="17">P4/O4-1</f>
+        <v>0.19426026330464774</v>
+      </c>
+      <c r="Q24" s="38">
+        <f t="shared" si="17"/>
+        <v>0.2464935449630965</v>
+      </c>
+      <c r="R24" s="38">
+        <f t="shared" si="17"/>
+        <v>0.15066760138121227</v>
+      </c>
+      <c r="S24" s="38">
+        <f t="shared" si="17"/>
+        <v>9.3822238221378251E-2</v>
+      </c>
       <c r="T24" s="38">
         <f>T4/S4-1</f>
         <v>0.25909722774006405</v>
@@ -2962,16 +3133,32 @@
       <c r="B27" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="O27" s="37">
+        <f t="shared" ref="O27:P27" si="18">O6/O4</f>
+        <v>0.34541698091422091</v>
+      </c>
+      <c r="P27" s="37">
+        <f t="shared" ref="P27:Q27" si="19">P6/P4</f>
+        <v>0.34736902734236785</v>
+      </c>
+      <c r="Q27" s="37">
+        <f t="shared" ref="Q27:S27" si="20">Q6/Q4</f>
+        <v>0.33958489696686456</v>
+      </c>
+      <c r="R27" s="37">
+        <f t="shared" si="20"/>
+        <v>0.34122585724960164</v>
+      </c>
       <c r="S27" s="37">
-        <f t="shared" ref="S27:T27" si="13">S6/S4</f>
+        <f t="shared" ref="S27:T27" si="21">S6/S4</f>
         <v>0.33639596505678548</v>
       </c>
       <c r="T27" s="37">
-        <f t="shared" ref="T27:U27" si="14">T6/T4</f>
+        <f t="shared" ref="T27:U27" si="22">T6/T4</f>
         <v>0.36863431168871746</v>
       </c>
       <c r="U27" s="37">
-        <f t="shared" ref="U27:V27" si="15">U6/U4</f>
+        <f t="shared" ref="U27:V27" si="23">U6/U4</f>
         <v>0.37491975176546116</v>
       </c>
       <c r="V27" s="37">
@@ -2986,37 +3173,70 @@
       <c r="B28" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="O28" s="37">
+        <f t="shared" ref="O28:P28" si="24">O8/O4</f>
+        <v>8.5733447649837827E-2</v>
+      </c>
+      <c r="P28" s="37">
+        <f t="shared" ref="P28:Q28" si="25">P8/P4</f>
+        <v>8.4134761751952072E-2</v>
+      </c>
+      <c r="Q28" s="37">
+        <f t="shared" ref="Q28:S28" si="26">Q8/Q4</f>
+        <v>7.9148076342942617E-2</v>
+      </c>
+      <c r="R28" s="37">
+        <f t="shared" si="26"/>
+        <v>7.5884570869648157E-2</v>
+      </c>
       <c r="S28" s="37">
-        <f t="shared" ref="S28:T28" si="16">S8/S4</f>
+        <f t="shared" ref="S28:T28" si="27">S8/S4</f>
         <v>8.7274645872553722E-2</v>
       </c>
       <c r="T28" s="37">
-        <f t="shared" ref="T28:U28" si="17">T8/T4</f>
+        <f t="shared" ref="T28:U28" si="28">T8/T4</f>
         <v>0.12775665557620919</v>
       </c>
       <c r="U28" s="37">
-        <f t="shared" ref="U28:V28" si="18">U8/U4</f>
+        <f t="shared" ref="U28:V28" si="29">U8/U4</f>
         <v>0.13053712818317997</v>
       </c>
       <c r="V28" s="37">
         <f>V8/V4</f>
         <v>0.1075657234597632</v>
       </c>
+      <c r="W28" s="90"/>
     </row>
     <row r="29" spans="2:23" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="O29" s="37">
+        <f t="shared" ref="O29:P29" si="30">O16/O4</f>
+        <v>6.1357500300940733E-2</v>
+      </c>
+      <c r="P29" s="37">
+        <f t="shared" ref="P29:Q29" si="31">P16/P4</f>
+        <v>5.8006055968337737E-2</v>
+      </c>
+      <c r="Q29" s="37">
+        <f t="shared" ref="Q29:S29" si="32">Q16/Q4</f>
+        <v>6.1205649742128443E-2</v>
+      </c>
+      <c r="R29" s="37">
+        <f t="shared" si="32"/>
+        <v>5.7984479225079918E-2</v>
+      </c>
       <c r="S29" s="37">
-        <f t="shared" ref="S29:T29" si="19">S16/S4</f>
+        <f t="shared" ref="S29:T29" si="33">S16/S4</f>
         <v>5.1077165784642366E-2</v>
       </c>
       <c r="T29" s="37">
-        <f t="shared" ref="T29:U29" si="20">T16/T4</f>
+        <f t="shared" ref="T29:U29" si="34">T16/T4</f>
         <v>8.9161863405134975E-2</v>
       </c>
       <c r="U29" s="37">
-        <f t="shared" ref="U29:V29" si="21">U16/U4</f>
+        <f t="shared" ref="U29:V29" si="35">U16/U4</f>
         <v>9.030601326770811E-2</v>
       </c>
       <c r="V29" s="37">
@@ -3028,16 +3248,32 @@
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="O30" s="37">
+        <f t="shared" ref="O30:P30" si="36">O15/O14</f>
+        <v>0.18711147274206652</v>
+      </c>
+      <c r="P30" s="37">
+        <f t="shared" ref="P30:Q30" si="37">P15/P14</f>
+        <v>0.21617429591167373</v>
+      </c>
+      <c r="Q30" s="37">
+        <f t="shared" ref="Q30:S30" si="38">Q15/Q14</f>
+        <v>0.19004420140466105</v>
+      </c>
+      <c r="R30" s="37">
+        <f t="shared" si="38"/>
+        <v>0.18771798704534129</v>
+      </c>
       <c r="S30" s="37">
-        <f t="shared" ref="S30:T30" si="22">S15/S14</f>
+        <f t="shared" ref="S30:T30" si="39">S15/S14</f>
         <v>0.22714593509322561</v>
       </c>
       <c r="T30" s="37">
-        <f t="shared" ref="T30:U30" si="23">T15/T14</f>
+        <f t="shared" ref="T30:U30" si="40">T15/T14</f>
         <v>0.18524509981177636</v>
       </c>
       <c r="U30" s="37">
-        <f t="shared" ref="U30:V30" si="24">U15/U14</f>
+        <f t="shared" ref="U30:V30" si="41">U15/U14</f>
         <v>0.19619047619047619</v>
       </c>
       <c r="V30" s="37">
@@ -3060,35 +3296,35 @@
       <c r="J34" s="70"/>
       <c r="L34" s="70"/>
       <c r="O34" s="32">
-        <f t="shared" ref="O34:U34" si="25">+O35+O38</f>
+        <f t="shared" ref="O34:S34" si="42">+O35+O38+O40</f>
         <v>0</v>
       </c>
       <c r="P34" s="32">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="42"/>
+        <v>648</v>
       </c>
       <c r="Q34" s="32">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="42"/>
+        <v>927</v>
       </c>
       <c r="R34" s="32">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="42"/>
+        <v>1093</v>
       </c>
       <c r="S34" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="42"/>
         <v>1050</v>
       </c>
       <c r="T34" s="32">
-        <f t="shared" si="25"/>
+        <f>+T35+T38+T40</f>
         <v>1091</v>
       </c>
       <c r="U34" s="32">
-        <f t="shared" si="25"/>
+        <f t="shared" ref="U34:V34" si="43">+U35+U38+U40</f>
         <v>1119</v>
       </c>
       <c r="V34" s="32">
-        <f>+V35+V38</f>
+        <f t="shared" si="43"/>
         <v>1140</v>
       </c>
       <c r="W34" s="84"/>
@@ -3103,31 +3339,31 @@
       <c r="J35" s="71"/>
       <c r="L35" s="71"/>
       <c r="O35" s="33">
-        <f t="shared" ref="O35:U35" si="26">SUM(O36:O37)</f>
+        <f t="shared" ref="O35:U35" si="44">SUM(O36:O37)</f>
         <v>0</v>
       </c>
       <c r="P35" s="33">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>573</v>
       </c>
       <c r="Q35" s="33">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>576</v>
       </c>
       <c r="R35" s="33">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>716</v>
       </c>
       <c r="S35" s="33">
-        <f t="shared" si="26"/>
+        <f t="shared" si="44"/>
         <v>757</v>
       </c>
       <c r="T35" s="33">
-        <f t="shared" si="26"/>
+        <f t="shared" si="44"/>
         <v>785</v>
       </c>
       <c r="U35" s="33">
-        <f t="shared" si="26"/>
+        <f t="shared" si="44"/>
         <v>808</v>
       </c>
       <c r="V35" s="33">
@@ -3145,6 +3381,15 @@
       <c r="H36" s="71"/>
       <c r="J36" s="71"/>
       <c r="L36" s="71"/>
+      <c r="P36" s="33">
+        <v>573</v>
+      </c>
+      <c r="Q36" s="33">
+        <v>576</v>
+      </c>
+      <c r="R36" s="33">
+        <v>620</v>
+      </c>
       <c r="S36" s="33">
         <v>656</v>
       </c>
@@ -3168,6 +3413,15 @@
       <c r="H37" s="71"/>
       <c r="J37" s="71"/>
       <c r="L37" s="71"/>
+      <c r="P37" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="33">
+        <v>0</v>
+      </c>
+      <c r="R37" s="33">
+        <v>96</v>
+      </c>
       <c r="S37" s="33">
         <v>101</v>
       </c>
@@ -3192,31 +3446,31 @@
       <c r="J38" s="71"/>
       <c r="L38" s="71"/>
       <c r="O38" s="33">
-        <f t="shared" ref="O38:U38" si="27">+O39</f>
+        <f t="shared" ref="O38:U38" si="45">+O39</f>
         <v>0</v>
       </c>
       <c r="P38" s="33">
-        <f t="shared" si="27"/>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Q38" s="33">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>265</v>
       </c>
       <c r="R38" s="33">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f t="shared" si="45"/>
+        <v>281</v>
       </c>
       <c r="S38" s="33">
-        <f t="shared" si="27"/>
+        <f t="shared" si="45"/>
         <v>293</v>
       </c>
       <c r="T38" s="33">
-        <f t="shared" si="27"/>
+        <f t="shared" si="45"/>
         <v>306</v>
       </c>
       <c r="U38" s="33">
-        <f t="shared" si="27"/>
+        <f t="shared" si="45"/>
         <v>311</v>
       </c>
       <c r="V38" s="33">
@@ -3234,6 +3488,15 @@
       <c r="H39" s="71"/>
       <c r="J39" s="71"/>
       <c r="L39" s="71"/>
+      <c r="P39" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="33">
+        <v>265</v>
+      </c>
+      <c r="R39" s="33">
+        <v>281</v>
+      </c>
       <c r="S39" s="33">
         <v>293</v>
       </c>
@@ -3248,370 +3511,466 @@
       </c>
       <c r="W39" s="54"/>
     </row>
-    <row r="40" spans="2:23" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="60" t="s">
+    <row r="40" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="71"/>
+      <c r="F40" s="71"/>
+      <c r="H40" s="71"/>
+      <c r="J40" s="71"/>
+      <c r="L40" s="71"/>
+      <c r="O40" s="33">
+        <f t="shared" ref="O40:R40" si="46">O41</f>
+        <v>0</v>
+      </c>
+      <c r="P40" s="33">
+        <f t="shared" si="46"/>
+        <v>75</v>
+      </c>
+      <c r="Q40" s="33">
+        <f t="shared" si="46"/>
+        <v>86</v>
+      </c>
+      <c r="R40" s="33">
+        <f t="shared" si="46"/>
+        <v>96</v>
+      </c>
+      <c r="S40" s="33">
+        <f>S41</f>
+        <v>0</v>
+      </c>
+      <c r="T40" s="33">
+        <f t="shared" ref="T40:V40" si="47">T41</f>
+        <v>0</v>
+      </c>
+      <c r="U40" s="33">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="V40" s="33">
+        <f t="shared" si="47"/>
+        <v>0</v>
+      </c>
+      <c r="W40" s="54"/>
+    </row>
+    <row r="41" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="71"/>
+      <c r="F41" s="71"/>
+      <c r="H41" s="71"/>
+      <c r="J41" s="71"/>
+      <c r="L41" s="71"/>
+      <c r="P41" s="33">
+        <v>75</v>
+      </c>
+      <c r="Q41" s="33">
+        <v>86</v>
+      </c>
+      <c r="R41" s="33">
+        <v>96</v>
+      </c>
+      <c r="S41" s="33">
+        <v>0</v>
+      </c>
+      <c r="T41" s="33">
+        <v>0</v>
+      </c>
+      <c r="U41" s="33">
+        <v>0</v>
+      </c>
+      <c r="V41" s="33">
+        <v>0</v>
+      </c>
+      <c r="W41" s="54"/>
+    </row>
+    <row r="42" spans="2:23" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="D40" s="72"/>
-      <c r="F40" s="72"/>
-      <c r="H40" s="72"/>
-      <c r="J40" s="72"/>
-      <c r="L40" s="72"/>
-      <c r="T40" s="61">
+      <c r="D42" s="72"/>
+      <c r="F42" s="72"/>
+      <c r="H42" s="72"/>
+      <c r="J42" s="72"/>
+      <c r="L42" s="72"/>
+      <c r="Q42" s="61">
+        <f>Q34-P34</f>
+        <v>279</v>
+      </c>
+      <c r="R42" s="61">
+        <f>R34-Q34</f>
+        <v>166</v>
+      </c>
+      <c r="S42" s="61">
+        <f>S34-R34</f>
+        <v>-43</v>
+      </c>
+      <c r="T42" s="61">
         <f>T34-S34</f>
         <v>41</v>
       </c>
-      <c r="U40" s="61">
-        <f t="shared" ref="U40:V40" si="28">U34-T34</f>
+      <c r="U42" s="61">
+        <f t="shared" ref="U42:V42" si="48">U34-T34</f>
         <v>28</v>
       </c>
-      <c r="V40" s="61">
-        <f t="shared" si="28"/>
+      <c r="V42" s="61">
+        <f t="shared" si="48"/>
         <v>21</v>
       </c>
-      <c r="W40" s="85"/>
-    </row>
-    <row r="41" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="33"/>
-      <c r="D41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="H41" s="70"/>
-      <c r="J41" s="70"/>
-      <c r="L41" s="70"/>
-      <c r="W41" s="84"/>
-    </row>
-    <row r="42" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="32" t="s">
+      <c r="W42" s="85"/>
+    </row>
+    <row r="43" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="33"/>
+      <c r="D43" s="70"/>
+      <c r="F43" s="70"/>
+      <c r="H43" s="70"/>
+      <c r="J43" s="70"/>
+      <c r="L43" s="70"/>
+      <c r="T43" s="32">
+        <v>0</v>
+      </c>
+      <c r="W43" s="84"/>
+    </row>
+    <row r="44" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="D42" s="70"/>
-      <c r="F42" s="70"/>
-      <c r="H42" s="70"/>
-      <c r="J42" s="70"/>
-      <c r="L42" s="70"/>
-      <c r="O42" s="32">
-        <f t="shared" ref="O42:U42" si="29">O43+O46</f>
-        <v>0</v>
-      </c>
-      <c r="P42" s="32">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="Q42" s="32">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="R42" s="32">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="S42" s="32">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="T42" s="32">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="U42" s="32">
-        <f t="shared" si="29"/>
-        <v>0</v>
-      </c>
-      <c r="V42" s="32">
-        <f>V43+V46</f>
+      <c r="D44" s="70"/>
+      <c r="F44" s="70"/>
+      <c r="H44" s="70"/>
+      <c r="J44" s="70"/>
+      <c r="L44" s="70"/>
+      <c r="O44" s="32">
+        <f t="shared" ref="O44:U44" si="49">O45+O48</f>
+        <v>0</v>
+      </c>
+      <c r="P44" s="32">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="32">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="R44" s="32">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="S44" s="32">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="T44" s="32">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="U44" s="32">
+        <f t="shared" si="49"/>
+        <v>0</v>
+      </c>
+      <c r="V44" s="32">
+        <f>V45+V48</f>
         <v>39484</v>
       </c>
-      <c r="W42" s="84"/>
-    </row>
-    <row r="43" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="47" t="s">
+      <c r="W44" s="84"/>
+    </row>
+    <row r="45" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D43" s="71"/>
-      <c r="F43" s="71"/>
-      <c r="H43" s="71"/>
-      <c r="J43" s="71"/>
-      <c r="L43" s="71"/>
-      <c r="O43" s="33">
-        <f t="shared" ref="O43:U43" si="30">SUM(O44:O45)</f>
-        <v>0</v>
-      </c>
-      <c r="P43" s="33">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="Q43" s="33">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="R43" s="33">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="S43" s="33">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="T43" s="33">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="U43" s="33">
-        <f t="shared" si="30"/>
-        <v>0</v>
-      </c>
-      <c r="V43" s="33">
-        <f>SUM(V44:V45)</f>
+      <c r="D45" s="71"/>
+      <c r="F45" s="71"/>
+      <c r="H45" s="71"/>
+      <c r="J45" s="71"/>
+      <c r="L45" s="71"/>
+      <c r="O45" s="33">
+        <f t="shared" ref="O45:U45" si="50">SUM(O46:O47)</f>
+        <v>0</v>
+      </c>
+      <c r="P45" s="33">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="Q45" s="33">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="R45" s="33">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="S45" s="33">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="T45" s="33">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="U45" s="33">
+        <f t="shared" si="50"/>
+        <v>0</v>
+      </c>
+      <c r="V45" s="33">
+        <f>SUM(V46:V47)</f>
         <v>34145</v>
       </c>
-      <c r="W43" s="54"/>
-    </row>
-    <row r="44" spans="2:23" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="48" t="s">
+      <c r="W45" s="54"/>
+    </row>
+    <row r="46" spans="2:23" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="D44" s="73"/>
-      <c r="F44" s="73"/>
-      <c r="H44" s="73"/>
-      <c r="J44" s="73"/>
-      <c r="L44" s="73"/>
-      <c r="V44" s="49">
+      <c r="D46" s="73"/>
+      <c r="F46" s="73"/>
+      <c r="H46" s="73"/>
+      <c r="J46" s="73"/>
+      <c r="L46" s="73"/>
+      <c r="V46" s="49">
         <v>33156</v>
       </c>
-      <c r="W44" s="54"/>
-    </row>
-    <row r="45" spans="2:23" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="48" t="s">
+      <c r="W46" s="54"/>
+    </row>
+    <row r="47" spans="2:23" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="D45" s="73"/>
-      <c r="F45" s="73"/>
-      <c r="H45" s="73"/>
-      <c r="J45" s="73"/>
-      <c r="L45" s="73"/>
-      <c r="V45" s="49">
+      <c r="D47" s="73"/>
+      <c r="F47" s="73"/>
+      <c r="H47" s="73"/>
+      <c r="J47" s="73"/>
+      <c r="L47" s="73"/>
+      <c r="V47" s="49">
         <v>989</v>
       </c>
-      <c r="W45" s="54"/>
-    </row>
-    <row r="46" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="47" t="s">
+      <c r="W47" s="54"/>
+    </row>
+    <row r="48" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D46" s="71"/>
-      <c r="F46" s="71"/>
-      <c r="H46" s="71"/>
-      <c r="J46" s="71"/>
-      <c r="L46" s="71"/>
-      <c r="O46" s="33">
-        <f t="shared" ref="O46:U46" si="31">O47</f>
-        <v>0</v>
-      </c>
-      <c r="P46" s="33">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="Q46" s="33">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="R46" s="33">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="S46" s="33">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="T46" s="33">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="U46" s="33">
-        <f t="shared" si="31"/>
-        <v>0</v>
-      </c>
-      <c r="V46" s="33">
-        <f>V47</f>
+      <c r="D48" s="71"/>
+      <c r="F48" s="71"/>
+      <c r="H48" s="71"/>
+      <c r="J48" s="71"/>
+      <c r="L48" s="71"/>
+      <c r="O48" s="33">
+        <f t="shared" ref="O48:U48" si="51">O49</f>
+        <v>0</v>
+      </c>
+      <c r="P48" s="33">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="Q48" s="33">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="R48" s="33">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="S48" s="33">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="T48" s="33">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="U48" s="33">
+        <f t="shared" si="51"/>
+        <v>0</v>
+      </c>
+      <c r="V48" s="33">
+        <f>V49</f>
         <v>5339</v>
       </c>
-      <c r="W46" s="54"/>
-    </row>
-    <row r="47" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="48" t="s">
+      <c r="W48" s="54"/>
+    </row>
+    <row r="49" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="D47" s="71"/>
-      <c r="F47" s="71"/>
-      <c r="H47" s="71"/>
-      <c r="J47" s="71"/>
-      <c r="L47" s="71"/>
-      <c r="V47" s="33">
+      <c r="D49" s="71"/>
+      <c r="F49" s="71"/>
+      <c r="H49" s="71"/>
+      <c r="J49" s="71"/>
+      <c r="L49" s="71"/>
+      <c r="V49" s="33">
         <v>5339</v>
       </c>
-      <c r="W47" s="54"/>
-    </row>
-    <row r="48" spans="2:23" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B48" s="60" t="s">
+      <c r="W49" s="54"/>
+    </row>
+    <row r="50" spans="2:23" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="60" t="s">
         <v>77</v>
       </c>
-      <c r="D48" s="74"/>
-      <c r="F48" s="74"/>
-      <c r="H48" s="74"/>
-      <c r="J48" s="74"/>
-      <c r="L48" s="74"/>
-      <c r="W48" s="86"/>
-    </row>
-    <row r="52" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B52" s="39" t="s">
+      <c r="D50" s="74"/>
+      <c r="F50" s="74"/>
+      <c r="H50" s="74"/>
+      <c r="J50" s="74"/>
+      <c r="L50" s="74"/>
+      <c r="W50" s="86"/>
+    </row>
+    <row r="54" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B54" s="39" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="53" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B53" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="D53" s="71"/>
-      <c r="F53" s="71"/>
-      <c r="H53" s="71"/>
-      <c r="J53" s="71"/>
-      <c r="L53" s="71"/>
-      <c r="S53" s="33">
-        <f>921.911+119.696</f>
-        <v>1041.607</v>
-      </c>
-      <c r="T53" s="33">
-        <f>920.729+118.24</f>
-        <v>1038.9690000000001</v>
-      </c>
-      <c r="U53" s="33">
-        <f>920+120</f>
-        <v>1040</v>
-      </c>
-      <c r="V53" s="33">
-        <f>921+120</f>
-        <v>1041</v>
-      </c>
-      <c r="W53" s="54"/>
-    </row>
-    <row r="54" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B54" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="D54" s="71"/>
-      <c r="F54" s="71"/>
-      <c r="H54" s="71"/>
-      <c r="J54" s="71"/>
-      <c r="L54" s="71"/>
-      <c r="S54" s="33">
-        <v>312.19799999999998</v>
-      </c>
-      <c r="T54" s="33">
-        <v>336.36399999999998</v>
-      </c>
-      <c r="U54" s="33">
-        <v>363</v>
-      </c>
-      <c r="V54" s="33">
-        <v>380</v>
-      </c>
-      <c r="W54" s="54"/>
     </row>
     <row r="55" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B55" s="33" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D55" s="71"/>
       <c r="F55" s="71"/>
       <c r="H55" s="71"/>
       <c r="J55" s="71"/>
       <c r="L55" s="71"/>
+      <c r="O55" s="33">
+        <f>837.45+101.174</f>
+        <v>938.62400000000002</v>
+      </c>
+      <c r="P55" s="33">
+        <f>841.691+103.693</f>
+        <v>945.38400000000001</v>
+      </c>
+      <c r="Q55" s="33">
+        <f>929.718+120.962</f>
+        <v>1050.68</v>
+      </c>
+      <c r="R55" s="33">
+        <f>949.606+126.559</f>
+        <v>1076.165</v>
+      </c>
       <c r="S55" s="33">
-        <v>1086.6179999999999</v>
+        <f>921.911+119.696</f>
+        <v>1041.607</v>
       </c>
       <c r="T55" s="33">
-        <v>1070.5809999999999</v>
+        <f>920.729+118.24</f>
+        <v>1038.9690000000001</v>
       </c>
       <c r="U55" s="33">
-        <v>1066</v>
+        <f>920+120</f>
+        <v>1040</v>
       </c>
       <c r="V55" s="33">
-        <v>1056</v>
+        <f>921+120</f>
+        <v>1041</v>
       </c>
       <c r="W55" s="54"/>
     </row>
     <row r="56" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B56" s="33" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D56" s="71"/>
       <c r="F56" s="71"/>
       <c r="H56" s="71"/>
       <c r="J56" s="71"/>
       <c r="L56" s="71"/>
+      <c r="O56" s="33">
+        <v>138.05000000000001</v>
+      </c>
+      <c r="P56" s="33">
+        <v>165.74799999999999</v>
+      </c>
+      <c r="Q56" s="33">
+        <v>308.65300000000002</v>
+      </c>
+      <c r="R56" s="33">
+        <v>389.952</v>
+      </c>
       <c r="S56" s="33">
-        <v>5.7</v>
+        <v>312.19799999999998</v>
       </c>
       <c r="T56" s="33">
-        <v>4.4790000000000001</v>
+        <v>336.36399999999998</v>
       </c>
       <c r="U56" s="33">
-        <v>8</v>
+        <v>363</v>
       </c>
       <c r="V56" s="33">
-        <v>8</v>
+        <v>380</v>
       </c>
       <c r="W56" s="54"/>
     </row>
     <row r="57" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B57" s="33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D57" s="71"/>
       <c r="F57" s="71"/>
       <c r="H57" s="71"/>
       <c r="J57" s="71"/>
       <c r="L57" s="71"/>
+      <c r="O57" s="33">
+        <v>0</v>
+      </c>
+      <c r="P57" s="33">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="33">
+        <v>0</v>
+      </c>
+      <c r="R57" s="33">
+        <v>0</v>
+      </c>
       <c r="S57" s="33">
-        <v>7.5170000000000003</v>
+        <v>1086.6179999999999</v>
       </c>
       <c r="T57" s="33">
-        <v>7.0839999999999996</v>
+        <v>1070.5809999999999</v>
       </c>
       <c r="U57" s="33">
-        <v>7</v>
+        <v>1066</v>
       </c>
       <c r="V57" s="33">
-        <v>6</v>
+        <v>1056</v>
       </c>
       <c r="W57" s="54"/>
     </row>
     <row r="58" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B58" s="33" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D58" s="71"/>
       <c r="F58" s="71"/>
       <c r="H58" s="71"/>
       <c r="J58" s="71"/>
       <c r="L58" s="71"/>
+      <c r="O58" s="33">
+        <v>3.9950000000000001</v>
+      </c>
+      <c r="P58" s="33">
+        <v>5.6689999999999996</v>
+      </c>
+      <c r="Q58" s="33">
+        <v>5.14</v>
+      </c>
+      <c r="R58" s="33">
+        <v>6.92</v>
+      </c>
       <c r="S58" s="33">
-        <v>22.988</v>
+        <v>5.7</v>
       </c>
       <c r="T58" s="33">
-        <v>32.241999999999997</v>
+        <v>4.4790000000000001</v>
       </c>
       <c r="U58" s="33">
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="V58" s="33">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="W58" s="54"/>
     </row>
     <row r="59" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B59" s="33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D59" s="71"/>
       <c r="F59" s="71"/>
@@ -3619,157 +3978,217 @@
       <c r="J59" s="71"/>
       <c r="L59" s="71"/>
       <c r="O59" s="33">
-        <f t="shared" ref="O59:U59" si="32">SUM(O53:O58)</f>
-        <v>0</v>
+        <v>2.7709999999999999</v>
       </c>
       <c r="P59" s="33">
-        <f t="shared" si="32"/>
-        <v>0</v>
+        <v>2.4129999999999998</v>
       </c>
       <c r="Q59" s="33">
-        <f t="shared" si="32"/>
-        <v>0</v>
+        <v>3.1869999999999998</v>
       </c>
       <c r="R59" s="33">
-        <f t="shared" si="32"/>
-        <v>0</v>
+        <v>10.989000000000001</v>
       </c>
       <c r="S59" s="33">
-        <f t="shared" si="32"/>
+        <v>7.5170000000000003</v>
+      </c>
+      <c r="T59" s="33">
+        <v>7.0839999999999996</v>
+      </c>
+      <c r="U59" s="33">
+        <v>7</v>
+      </c>
+      <c r="V59" s="33">
+        <v>6</v>
+      </c>
+      <c r="W59" s="54"/>
+    </row>
+    <row r="60" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="D60" s="71"/>
+      <c r="F60" s="71"/>
+      <c r="H60" s="71"/>
+      <c r="J60" s="71"/>
+      <c r="L60" s="71"/>
+      <c r="O60" s="33">
+        <v>0.47299999999999998</v>
+      </c>
+      <c r="P60" s="33">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="Q60" s="33">
+        <v>5.6539999999999999</v>
+      </c>
+      <c r="R60" s="33">
+        <v>9.1950000000000003</v>
+      </c>
+      <c r="S60" s="33">
+        <v>22.988</v>
+      </c>
+      <c r="T60" s="33">
+        <v>32.241999999999997</v>
+      </c>
+      <c r="U60" s="33">
+        <v>31</v>
+      </c>
+      <c r="V60" s="33">
+        <v>30</v>
+      </c>
+      <c r="W60" s="54"/>
+    </row>
+    <row r="61" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D61" s="71"/>
+      <c r="F61" s="71"/>
+      <c r="H61" s="71"/>
+      <c r="J61" s="71"/>
+      <c r="L61" s="71"/>
+      <c r="O61" s="33">
+        <f t="shared" ref="O61:U61" si="52">SUM(O55:O60)</f>
+        <v>1083.9129999999998</v>
+      </c>
+      <c r="P61" s="33">
+        <f t="shared" si="52"/>
+        <v>1120.0380000000002</v>
+      </c>
+      <c r="Q61" s="33">
+        <f t="shared" si="52"/>
+        <v>1373.3140000000001</v>
+      </c>
+      <c r="R61" s="33">
+        <f t="shared" si="52"/>
+        <v>1493.221</v>
+      </c>
+      <c r="S61" s="33">
+        <f t="shared" si="52"/>
         <v>2476.6279999999992</v>
       </c>
-      <c r="T59" s="33">
-        <f t="shared" si="32"/>
+      <c r="T61" s="33">
+        <f t="shared" si="52"/>
         <v>2489.7189999999996</v>
       </c>
-      <c r="U59" s="33">
-        <f t="shared" si="32"/>
+      <c r="U61" s="33">
+        <f t="shared" si="52"/>
         <v>2515</v>
       </c>
-      <c r="V59" s="33">
-        <f>SUM(V53:V58)</f>
+      <c r="V61" s="33">
+        <f>SUM(V55:V60)</f>
         <v>2521</v>
       </c>
-      <c r="W59" s="54"/>
-    </row>
-    <row r="60" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B60" s="32" t="s">
+      <c r="W61" s="54"/>
+    </row>
+    <row r="62" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="D60" s="70"/>
-      <c r="F60" s="70"/>
-      <c r="H60" s="70"/>
-      <c r="J60" s="70"/>
-      <c r="L60" s="70"/>
-      <c r="S60" s="32">
+      <c r="D62" s="70"/>
+      <c r="F62" s="70"/>
+      <c r="H62" s="70"/>
+      <c r="J62" s="70"/>
+      <c r="L62" s="70"/>
+      <c r="O62" s="32">
+        <v>91.147999999999996</v>
+      </c>
+      <c r="P62" s="32">
+        <v>155.511</v>
+      </c>
+      <c r="Q62" s="32">
+        <v>90.816000000000003</v>
+      </c>
+      <c r="R62" s="32">
+        <v>86.201999999999998</v>
+      </c>
+      <c r="S62" s="32">
         <v>428.20499999999998</v>
       </c>
-      <c r="T60" s="32">
+      <c r="T62" s="32">
         <v>217.68199999999999</v>
       </c>
-      <c r="U60" s="32">
+      <c r="U62" s="32">
         <v>173</v>
       </c>
-      <c r="V60" s="32">
+      <c r="V62" s="32">
         <v>237</v>
       </c>
-      <c r="W60" s="84"/>
-    </row>
-    <row r="61" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="32" t="s">
+      <c r="W62" s="84"/>
+    </row>
+    <row r="63" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="D61" s="70"/>
-      <c r="F61" s="70"/>
-      <c r="H61" s="70"/>
-      <c r="J61" s="70"/>
-      <c r="L61" s="70"/>
-      <c r="S61" s="32">
+      <c r="D63" s="70"/>
+      <c r="F63" s="70"/>
+      <c r="H63" s="70"/>
+      <c r="J63" s="70"/>
+      <c r="L63" s="70"/>
+      <c r="O63" s="32">
+        <v>356.31200000000001</v>
+      </c>
+      <c r="P63" s="32">
+        <v>462.11900000000003</v>
+      </c>
+      <c r="Q63" s="32">
+        <v>558.69000000000005</v>
+      </c>
+      <c r="R63" s="32">
+        <v>670.721</v>
+      </c>
+      <c r="S63" s="32">
         <v>588</v>
       </c>
-      <c r="T61" s="32">
+      <c r="T63" s="32">
         <v>605.12599999999998</v>
       </c>
-      <c r="U61" s="32">
+      <c r="U63" s="32">
         <v>863</v>
       </c>
-      <c r="V61" s="32">
+      <c r="V63" s="32">
         <v>764</v>
       </c>
-      <c r="W61" s="84"/>
-    </row>
-    <row r="62" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="33" t="s">
+      <c r="W63" s="84"/>
+    </row>
+    <row r="64" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="D62" s="71"/>
-      <c r="F62" s="71"/>
-      <c r="H62" s="71"/>
-      <c r="J62" s="71"/>
-      <c r="L62" s="71"/>
-      <c r="S62" s="33">
+      <c r="D64" s="71"/>
+      <c r="F64" s="71"/>
+      <c r="H64" s="71"/>
+      <c r="J64" s="71"/>
+      <c r="L64" s="71"/>
+      <c r="O64" s="33">
+        <v>28.760999999999999</v>
+      </c>
+      <c r="P64" s="33">
+        <v>35.398000000000003</v>
+      </c>
+      <c r="Q64" s="33">
+        <v>34.042000000000002</v>
+      </c>
+      <c r="R64" s="33">
+        <v>71.64</v>
+      </c>
+      <c r="S64" s="33">
         <v>60.588000000000001</v>
       </c>
-      <c r="T62" s="33">
+      <c r="T64" s="33">
         <v>42.16</v>
       </c>
-      <c r="U62" s="33">
+      <c r="U64" s="33">
         <v>53</v>
       </c>
-      <c r="V62" s="33">
+      <c r="V64" s="33">
         <v>52</v>
       </c>
-      <c r="W62" s="54"/>
-    </row>
-    <row r="63" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B63" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="D63" s="71"/>
-      <c r="F63" s="71"/>
-      <c r="H63" s="71"/>
-      <c r="J63" s="71"/>
-      <c r="L63" s="71"/>
-      <c r="S63" s="33">
-        <v>0</v>
-      </c>
-      <c r="T63" s="33">
-        <v>0</v>
-      </c>
-      <c r="U63" s="33">
-        <v>9</v>
-      </c>
-      <c r="V63" s="33">
-        <v>12</v>
-      </c>
-      <c r="W63" s="54"/>
-    </row>
-    <row r="64" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B64" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="D64" s="70"/>
-      <c r="F64" s="70"/>
-      <c r="H64" s="70"/>
-      <c r="J64" s="70"/>
-      <c r="L64" s="70"/>
-      <c r="S64" s="32">
-        <v>16.702000000000002</v>
-      </c>
-      <c r="T64" s="32">
-        <v>3.7669999999999999</v>
-      </c>
-      <c r="U64" s="32">
-        <v>25</v>
-      </c>
-      <c r="V64" s="32">
-        <v>1</v>
-      </c>
-      <c r="W64" s="84"/>
+      <c r="W64" s="54"/>
     </row>
     <row r="65" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B65" s="33" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="D65" s="71"/>
       <c r="F65" s="71"/>
@@ -3777,143 +4196,198 @@
       <c r="J65" s="71"/>
       <c r="L65" s="71"/>
       <c r="O65" s="33">
-        <f t="shared" ref="O65:U65" si="33">SUM(O59:O64)</f>
         <v>0</v>
       </c>
       <c r="P65" s="33">
-        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="Q65" s="33">
-        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="R65" s="33">
-        <f t="shared" si="33"/>
-        <v>0</v>
+        <v>6.2939999999999996</v>
       </c>
       <c r="S65" s="33">
-        <f t="shared" si="33"/>
+        <v>0</v>
+      </c>
+      <c r="T65" s="33">
+        <v>0</v>
+      </c>
+      <c r="U65" s="33">
+        <v>9</v>
+      </c>
+      <c r="V65" s="33">
+        <v>12</v>
+      </c>
+      <c r="W65" s="54"/>
+    </row>
+    <row r="66" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D66" s="70"/>
+      <c r="F66" s="70"/>
+      <c r="H66" s="70"/>
+      <c r="J66" s="70"/>
+      <c r="L66" s="70"/>
+      <c r="O66" s="32">
+        <v>4.7690000000000001</v>
+      </c>
+      <c r="P66" s="32">
+        <v>0.41</v>
+      </c>
+      <c r="Q66" s="32">
+        <v>0</v>
+      </c>
+      <c r="R66" s="32">
+        <v>3.7810000000000001</v>
+      </c>
+      <c r="S66" s="32">
+        <v>16.702000000000002</v>
+      </c>
+      <c r="T66" s="32">
+        <v>3.7669999999999999</v>
+      </c>
+      <c r="U66" s="32">
+        <v>25</v>
+      </c>
+      <c r="V66" s="32">
+        <v>1</v>
+      </c>
+      <c r="W66" s="84"/>
+    </row>
+    <row r="67" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D67" s="71"/>
+      <c r="F67" s="71"/>
+      <c r="H67" s="71"/>
+      <c r="J67" s="71"/>
+      <c r="L67" s="71"/>
+      <c r="O67" s="33">
+        <f t="shared" ref="O67:U67" si="53">SUM(O61:O66)</f>
+        <v>1564.9029999999996</v>
+      </c>
+      <c r="P67" s="33">
+        <f t="shared" si="53"/>
+        <v>1773.4760000000001</v>
+      </c>
+      <c r="Q67" s="33">
+        <f t="shared" si="53"/>
+        <v>2056.8620000000001</v>
+      </c>
+      <c r="R67" s="33">
+        <f t="shared" si="53"/>
+        <v>2331.8589999999999</v>
+      </c>
+      <c r="S67" s="33">
+        <f t="shared" si="53"/>
         <v>3570.1229999999996</v>
       </c>
-      <c r="T65" s="33">
-        <f t="shared" si="33"/>
+      <c r="T67" s="33">
+        <f t="shared" si="53"/>
         <v>3358.4539999999988</v>
       </c>
-      <c r="U65" s="33">
-        <f t="shared" si="33"/>
+      <c r="U67" s="33">
+        <f t="shared" si="53"/>
         <v>3638</v>
       </c>
-      <c r="V65" s="33">
-        <f>SUM(V59:V64)</f>
+      <c r="V67" s="33">
+        <f>SUM(V61:V66)</f>
         <v>3587</v>
       </c>
-      <c r="W65" s="54"/>
-    </row>
-    <row r="66" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D66" s="71"/>
-      <c r="F66" s="71"/>
-      <c r="H66" s="71"/>
-      <c r="J66" s="71"/>
-      <c r="L66" s="71"/>
-      <c r="W66" s="54"/>
-    </row>
-    <row r="67" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D67" s="70"/>
-      <c r="F67" s="70"/>
-      <c r="H67" s="70"/>
-      <c r="J67" s="70"/>
-      <c r="L67" s="70"/>
-      <c r="S67" s="32">
-        <v>561.41800000000001</v>
-      </c>
-      <c r="T67" s="32">
-        <v>723.73599999999999</v>
-      </c>
-      <c r="U67" s="32">
-        <v>950</v>
-      </c>
-      <c r="V67" s="32">
-        <v>873</v>
-      </c>
-      <c r="W67" s="84"/>
+      <c r="W67" s="54"/>
     </row>
     <row r="68" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B68" s="33" t="s">
-        <v>94</v>
-      </c>
       <c r="D68" s="71"/>
       <c r="F68" s="71"/>
       <c r="H68" s="71"/>
       <c r="J68" s="71"/>
       <c r="L68" s="71"/>
-      <c r="S68" s="33">
-        <f>1146.233+0.171</f>
-        <v>1146.404</v>
-      </c>
-      <c r="T68" s="33">
-        <v>1138.634</v>
-      </c>
-      <c r="U68" s="33">
-        <v>1140</v>
-      </c>
-      <c r="V68" s="33">
-        <v>1124</v>
-      </c>
       <c r="W68" s="54"/>
     </row>
-    <row r="69" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B69" s="33" t="s">
-        <v>85</v>
-      </c>
-      <c r="D69" s="71"/>
-      <c r="F69" s="71"/>
-      <c r="H69" s="71"/>
-      <c r="J69" s="71"/>
-      <c r="L69" s="71"/>
-      <c r="S69" s="33">
-        <v>29.007999999999999</v>
-      </c>
-      <c r="T69" s="33">
-        <v>27.475999999999999</v>
-      </c>
-      <c r="U69" s="33">
-        <v>43</v>
-      </c>
-      <c r="V69" s="33">
-        <v>43</v>
-      </c>
-      <c r="W69" s="54"/>
+    <row r="69" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D69" s="70"/>
+      <c r="F69" s="70"/>
+      <c r="H69" s="70"/>
+      <c r="J69" s="70"/>
+      <c r="L69" s="70"/>
+      <c r="O69" s="32">
+        <f>435.142+16.041</f>
+        <v>451.18299999999999</v>
+      </c>
+      <c r="P69" s="32">
+        <f>17.886+543.725</f>
+        <v>561.61099999999999</v>
+      </c>
+      <c r="Q69" s="32">
+        <f>558.426+19.209</f>
+        <v>577.63499999999999</v>
+      </c>
+      <c r="R69" s="32">
+        <v>562.94100000000003</v>
+      </c>
+      <c r="S69" s="32">
+        <v>561.41800000000001</v>
+      </c>
+      <c r="T69" s="32">
+        <v>723.73599999999999</v>
+      </c>
+      <c r="U69" s="32">
+        <v>950</v>
+      </c>
+      <c r="V69" s="32">
+        <v>873</v>
+      </c>
+      <c r="W69" s="84"/>
     </row>
     <row r="70" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B70" s="33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D70" s="71"/>
       <c r="F70" s="71"/>
       <c r="H70" s="71"/>
       <c r="J70" s="71"/>
       <c r="L70" s="71"/>
+      <c r="O70" s="33">
+        <f>4.252+66.544</f>
+        <v>70.795999999999992</v>
+      </c>
+      <c r="P70" s="33">
+        <f>76.961+6.469</f>
+        <v>83.429999999999993</v>
+      </c>
+      <c r="Q70" s="33">
+        <f>7.306+87.13</f>
+        <v>94.435999999999993</v>
+      </c>
+      <c r="R70" s="33">
+        <f>92.891+7.104</f>
+        <v>99.995000000000005</v>
+      </c>
       <c r="S70" s="33">
-        <v>0.76600000000000001</v>
+        <f>1146.233+0.171</f>
+        <v>1146.404</v>
       </c>
       <c r="T70" s="33">
-        <v>4.5110000000000001</v>
+        <v>1138.634</v>
       </c>
       <c r="U70" s="33">
-        <v>4</v>
+        <v>1140</v>
       </c>
       <c r="V70" s="33">
-        <v>3</v>
+        <v>1124</v>
       </c>
       <c r="W70" s="54"/>
     </row>
     <row r="71" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B71" s="33" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="D71" s="71"/>
       <c r="F71" s="71"/>
@@ -3921,182 +4395,256 @@
       <c r="J71" s="71"/>
       <c r="L71" s="71"/>
       <c r="O71" s="33">
-        <f t="shared" ref="O71:U71" si="34">SUM(O67:O70)</f>
-        <v>0</v>
+        <v>20.119</v>
       </c>
       <c r="P71" s="33">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <v>18.844999999999999</v>
       </c>
       <c r="Q71" s="33">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <v>24.495000000000001</v>
       </c>
       <c r="R71" s="33">
-        <f t="shared" si="34"/>
-        <v>0</v>
+        <v>27.148</v>
       </c>
       <c r="S71" s="33">
-        <f t="shared" si="34"/>
-        <v>1737.5960000000002</v>
+        <v>29.007999999999999</v>
       </c>
       <c r="T71" s="33">
-        <f t="shared" si="34"/>
-        <v>1894.357</v>
+        <v>27.475999999999999</v>
       </c>
       <c r="U71" s="33">
-        <f t="shared" si="34"/>
-        <v>2137</v>
+        <v>43</v>
       </c>
       <c r="V71" s="33">
-        <f>SUM(V67:V70)</f>
-        <v>2043</v>
+        <v>43</v>
       </c>
       <c r="W71" s="54"/>
     </row>
-    <row r="72" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" s="70"/>
-      <c r="F72" s="70"/>
-      <c r="H72" s="70"/>
-      <c r="J72" s="70"/>
-      <c r="L72" s="70"/>
-      <c r="S72" s="32">
-        <f>0.928+211.062</f>
-        <v>211.99</v>
-      </c>
-      <c r="T72" s="32">
-        <v>6.875</v>
-      </c>
-      <c r="U72" s="32">
-        <v>6</v>
-      </c>
-      <c r="V72" s="32">
-        <v>81</v>
-      </c>
-      <c r="W72" s="84"/>
+    <row r="72" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D72" s="71"/>
+      <c r="F72" s="71"/>
+      <c r="H72" s="71"/>
+      <c r="J72" s="71"/>
+      <c r="L72" s="71"/>
+      <c r="O72" s="33">
+        <v>2.0470000000000002</v>
+      </c>
+      <c r="P72" s="33">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="Q72" s="33">
+        <v>0.379</v>
+      </c>
+      <c r="R72" s="33">
+        <v>0.374</v>
+      </c>
+      <c r="S72" s="33">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="T72" s="33">
+        <v>4.5110000000000001</v>
+      </c>
+      <c r="U72" s="33">
+        <v>4</v>
+      </c>
+      <c r="V72" s="33">
+        <v>3</v>
+      </c>
+      <c r="W72" s="54"/>
     </row>
     <row r="73" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B73" s="33" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D73" s="71"/>
       <c r="F73" s="71"/>
       <c r="H73" s="71"/>
       <c r="J73" s="71"/>
       <c r="L73" s="71"/>
+      <c r="O73" s="33">
+        <f t="shared" ref="O73:U73" si="54">SUM(O69:O72)</f>
+        <v>544.1450000000001</v>
+      </c>
+      <c r="P73" s="33">
+        <f t="shared" si="54"/>
+        <v>664.80799999999999</v>
+      </c>
+      <c r="Q73" s="33">
+        <f t="shared" si="54"/>
+        <v>696.94500000000005</v>
+      </c>
+      <c r="R73" s="33">
+        <f t="shared" si="54"/>
+        <v>690.45800000000008</v>
+      </c>
       <c r="S73" s="33">
-        <v>419.99900000000002</v>
+        <f t="shared" si="54"/>
+        <v>1737.5960000000002</v>
       </c>
       <c r="T73" s="33">
-        <v>524.26</v>
+        <f t="shared" si="54"/>
+        <v>1894.357</v>
       </c>
       <c r="U73" s="33">
-        <v>564</v>
+        <f t="shared" si="54"/>
+        <v>2137</v>
       </c>
       <c r="V73" s="33">
-        <v>541</v>
+        <f>SUM(V69:V72)</f>
+        <v>2043</v>
       </c>
       <c r="W73" s="54"/>
     </row>
-    <row r="74" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="D74" s="71"/>
-      <c r="F74" s="71"/>
-      <c r="H74" s="71"/>
-      <c r="J74" s="71"/>
-      <c r="L74" s="71"/>
-      <c r="S74" s="33">
-        <v>149.011</v>
-      </c>
-      <c r="T74" s="33">
-        <v>162.73500000000001</v>
-      </c>
-      <c r="U74" s="33">
-        <v>170</v>
-      </c>
-      <c r="V74" s="33">
-        <v>177</v>
-      </c>
-      <c r="W74" s="54"/>
+    <row r="74" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="D74" s="70"/>
+      <c r="F74" s="70"/>
+      <c r="H74" s="70"/>
+      <c r="J74" s="70"/>
+      <c r="L74" s="70"/>
+      <c r="O74" s="32">
+        <v>0</v>
+      </c>
+      <c r="P74" s="32">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="32">
+        <f>47.212+6.112</f>
+        <v>53.324000000000005</v>
+      </c>
+      <c r="R74" s="32">
+        <f>5.646+124.272</f>
+        <v>129.91800000000001</v>
+      </c>
+      <c r="S74" s="32">
+        <f>0.928+211.062</f>
+        <v>211.99</v>
+      </c>
+      <c r="T74" s="32">
+        <v>6.875</v>
+      </c>
+      <c r="U74" s="32">
+        <v>6</v>
+      </c>
+      <c r="V74" s="32">
+        <v>81</v>
+      </c>
+      <c r="W74" s="84"/>
     </row>
     <row r="75" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B75" s="33" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D75" s="71"/>
       <c r="F75" s="71"/>
       <c r="H75" s="71"/>
       <c r="J75" s="71"/>
       <c r="L75" s="71"/>
+      <c r="O75" s="33">
+        <v>189.74299999999999</v>
+      </c>
+      <c r="P75" s="33">
+        <v>267.815</v>
+      </c>
+      <c r="Q75" s="33">
+        <v>336.072</v>
+      </c>
+      <c r="R75" s="33">
+        <v>395.96600000000001</v>
+      </c>
       <c r="S75" s="33">
-        <f>150.087+1.847</f>
-        <v>151.934</v>
+        <v>419.99900000000002</v>
       </c>
       <c r="T75" s="33">
-        <v>16.140999999999998</v>
+        <v>524.26</v>
       </c>
       <c r="U75" s="33">
-        <v>0</v>
+        <v>564</v>
       </c>
       <c r="V75" s="33">
-        <v>13</v>
+        <v>541</v>
       </c>
       <c r="W75" s="54"/>
     </row>
     <row r="76" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B76" s="33" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D76" s="71"/>
       <c r="F76" s="71"/>
       <c r="H76" s="71"/>
       <c r="J76" s="71"/>
       <c r="L76" s="71"/>
+      <c r="O76" s="33">
+        <v>1.119</v>
+      </c>
+      <c r="P76" s="33">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="Q76" s="33">
+        <v>1.87</v>
+      </c>
+      <c r="R76" s="33">
+        <v>3.63</v>
+      </c>
       <c r="S76" s="33">
-        <v>26.114999999999998</v>
+        <v>149.011</v>
       </c>
       <c r="T76" s="33">
-        <v>12.510999999999999</v>
+        <v>162.73500000000001</v>
       </c>
       <c r="U76" s="33">
-        <v>4</v>
+        <v>170</v>
       </c>
       <c r="V76" s="33">
-        <v>6</v>
+        <v>177</v>
       </c>
       <c r="W76" s="54"/>
     </row>
     <row r="77" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B77" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D77" s="71"/>
       <c r="F77" s="71"/>
       <c r="H77" s="71"/>
       <c r="J77" s="71"/>
       <c r="L77" s="71"/>
+      <c r="O77" s="33">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="P77" s="33">
+        <v>2.0699999999999998</v>
+      </c>
+      <c r="Q77" s="33">
+        <v>16.666</v>
+      </c>
+      <c r="R77" s="33">
+        <v>13.731</v>
+      </c>
       <c r="S77" s="33">
-        <v>6.0789999999999997</v>
+        <f>150.087+1.847</f>
+        <v>151.934</v>
       </c>
       <c r="T77" s="33">
-        <v>8.6069999999999993</v>
+        <v>16.140999999999998</v>
       </c>
       <c r="U77" s="33">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="V77" s="33">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="W77" s="54"/>
     </row>
     <row r="78" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B78" s="33" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D78" s="71"/>
       <c r="F78" s="71"/>
@@ -4104,224 +4652,300 @@
       <c r="J78" s="71"/>
       <c r="L78" s="71"/>
       <c r="O78" s="33">
-        <f t="shared" ref="O78:U78" si="35">SUM(O71:O77)</f>
-        <v>0</v>
+        <v>10.29</v>
       </c>
       <c r="P78" s="33">
-        <f t="shared" si="35"/>
-        <v>0</v>
+        <v>19.338999999999999</v>
       </c>
       <c r="Q78" s="33">
-        <f t="shared" si="35"/>
-        <v>0</v>
+        <v>19.677</v>
       </c>
       <c r="R78" s="33">
-        <f t="shared" si="35"/>
-        <v>0</v>
+        <v>23.196999999999999</v>
       </c>
       <c r="S78" s="33">
-        <f t="shared" si="35"/>
-        <v>2702.7240000000002</v>
+        <v>26.114999999999998</v>
       </c>
       <c r="T78" s="33">
-        <f t="shared" si="35"/>
-        <v>2625.4860000000003</v>
+        <v>12.510999999999999</v>
       </c>
       <c r="U78" s="33">
-        <f t="shared" si="35"/>
-        <v>2892</v>
+        <v>4</v>
       </c>
       <c r="V78" s="33">
-        <f>SUM(V71:V77)</f>
-        <v>2867</v>
+        <v>6</v>
       </c>
       <c r="W78" s="54"/>
     </row>
     <row r="79" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="33" t="s">
+        <v>97</v>
+      </c>
       <c r="D79" s="71"/>
       <c r="F79" s="71"/>
       <c r="H79" s="71"/>
       <c r="J79" s="71"/>
       <c r="L79" s="71"/>
+      <c r="O79" s="33">
+        <v>4.7690000000000001</v>
+      </c>
+      <c r="P79" s="33">
+        <v>4.8689999999999998</v>
+      </c>
+      <c r="Q79" s="33">
+        <v>6.2930000000000001</v>
+      </c>
+      <c r="R79" s="33">
+        <v>6.718</v>
+      </c>
+      <c r="S79" s="33">
+        <v>6.0789999999999997</v>
+      </c>
+      <c r="T79" s="33">
+        <v>8.6069999999999993</v>
+      </c>
+      <c r="U79" s="33">
+        <v>11</v>
+      </c>
+      <c r="V79" s="33">
+        <v>6</v>
+      </c>
       <c r="W79" s="54"/>
     </row>
     <row r="80" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B80" s="33" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D80" s="71"/>
       <c r="F80" s="71"/>
       <c r="H80" s="71"/>
       <c r="J80" s="71"/>
       <c r="L80" s="71"/>
+      <c r="O80" s="33">
+        <f>SUM(O73:O79)</f>
+        <v>750.55300000000011</v>
+      </c>
+      <c r="P80" s="33">
+        <f t="shared" ref="O80:U80" si="55">SUM(P73:P79)</f>
+        <v>959.8950000000001</v>
+      </c>
+      <c r="Q80" s="33">
+        <f t="shared" si="55"/>
+        <v>1130.8469999999995</v>
+      </c>
+      <c r="R80" s="33">
+        <f t="shared" si="55"/>
+        <v>1263.6180000000002</v>
+      </c>
       <c r="S80" s="33">
-        <v>867.399</v>
+        <f t="shared" si="55"/>
+        <v>2702.7240000000002</v>
       </c>
       <c r="T80" s="33">
-        <v>732.96799999999996</v>
+        <f t="shared" si="55"/>
+        <v>2625.4860000000003</v>
       </c>
       <c r="U80" s="33">
-        <v>746</v>
+        <f t="shared" si="55"/>
+        <v>2892</v>
       </c>
       <c r="V80" s="33">
-        <v>720</v>
+        <f>SUM(V73:V79)</f>
+        <v>2867</v>
       </c>
       <c r="W80" s="54"/>
     </row>
     <row r="81" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="33" t="s">
-        <v>101</v>
-      </c>
       <c r="D81" s="71"/>
       <c r="F81" s="71"/>
       <c r="H81" s="71"/>
       <c r="J81" s="71"/>
       <c r="L81" s="71"/>
-      <c r="S81" s="33">
-        <f>+S80+S78</f>
-        <v>3570.123</v>
-      </c>
-      <c r="T81" s="33">
-        <f>+T80+T78</f>
-        <v>3358.4540000000002</v>
-      </c>
-      <c r="U81" s="33">
-        <f>+U80+U78</f>
-        <v>3638</v>
-      </c>
-      <c r="V81" s="33">
-        <f>+V80+V78</f>
-        <v>3587</v>
-      </c>
       <c r="W81" s="54"/>
     </row>
     <row r="82" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="33" t="s">
+        <v>100</v>
+      </c>
       <c r="D82" s="71"/>
       <c r="F82" s="71"/>
       <c r="H82" s="71"/>
       <c r="J82" s="71"/>
       <c r="L82" s="71"/>
+      <c r="O82" s="33">
+        <v>814.35</v>
+      </c>
+      <c r="P82" s="33">
+        <v>813.62099999999998</v>
+      </c>
+      <c r="Q82" s="33">
+        <v>925.38499999999999</v>
+      </c>
+      <c r="R82" s="33">
+        <v>1068.241</v>
+      </c>
+      <c r="S82" s="33">
+        <v>867.399</v>
+      </c>
+      <c r="T82" s="33">
+        <v>732.96799999999996</v>
+      </c>
+      <c r="U82" s="33">
+        <v>746</v>
+      </c>
+      <c r="V82" s="33">
+        <v>720</v>
+      </c>
       <c r="W82" s="54"/>
     </row>
     <row r="83" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B83" s="33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D83" s="71"/>
       <c r="F83" s="71"/>
       <c r="H83" s="71"/>
       <c r="J83" s="71"/>
       <c r="L83" s="71"/>
+      <c r="O83" s="33">
+        <f t="shared" ref="O83:P83" si="56">+O82+O80</f>
+        <v>1564.9030000000002</v>
+      </c>
+      <c r="P83" s="33">
+        <f t="shared" si="56"/>
+        <v>1773.5160000000001</v>
+      </c>
+      <c r="Q83" s="33">
+        <f>+Q82+Q80</f>
+        <v>2056.2319999999995</v>
+      </c>
+      <c r="R83" s="33">
+        <f>+R82+R80</f>
+        <v>2331.8590000000004</v>
+      </c>
       <c r="S83" s="33">
-        <f t="shared" ref="S83:T83" si="36">S65-S78</f>
-        <v>867.39899999999943</v>
+        <f>+S82+S80</f>
+        <v>3570.123</v>
       </c>
       <c r="T83" s="33">
-        <f t="shared" ref="T83:U83" si="37">T65-T78</f>
-        <v>732.96799999999848</v>
+        <f>+T82+T80</f>
+        <v>3358.4540000000002</v>
       </c>
       <c r="U83" s="33">
-        <f t="shared" ref="U83:V83" si="38">U65-U78</f>
-        <v>746</v>
+        <f>+U82+U80</f>
+        <v>3638</v>
       </c>
       <c r="V83" s="33">
-        <f>V65-V78</f>
-        <v>720</v>
+        <f>+V82+V80</f>
+        <v>3587</v>
       </c>
       <c r="W83" s="54"/>
     </row>
-    <row r="84" spans="2:23" s="53" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="53" t="s">
-        <v>103</v>
-      </c>
-      <c r="D84" s="75"/>
-      <c r="F84" s="75"/>
-      <c r="H84" s="75"/>
-      <c r="J84" s="75"/>
-      <c r="L84" s="75"/>
-      <c r="S84" s="53">
-        <f t="shared" ref="S84" si="39">S83/S22</f>
-        <v>0.86690486422738977</v>
-      </c>
-      <c r="T84" s="53">
-        <f t="shared" ref="T84" si="40">T83/T22</f>
-        <v>0.73245894103597842</v>
-      </c>
-      <c r="U84" s="53">
-        <f>U83/U22</f>
-        <v>0.74520933289779545</v>
-      </c>
-      <c r="V84" s="53">
-        <f>V83/V22</f>
-        <v>0.71885486420132727</v>
-      </c>
-      <c r="W84" s="87"/>
+    <row r="84" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D84" s="71"/>
+      <c r="F84" s="71"/>
+      <c r="H84" s="71"/>
+      <c r="J84" s="71"/>
+      <c r="L84" s="71"/>
+      <c r="W84" s="54"/>
     </row>
     <row r="85" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B85" s="33" t="s">
+        <v>102</v>
+      </c>
       <c r="D85" s="71"/>
       <c r="F85" s="71"/>
       <c r="H85" s="71"/>
       <c r="J85" s="71"/>
       <c r="L85" s="71"/>
+      <c r="O85" s="33">
+        <f t="shared" ref="O85:Q85" si="57">O67-O80</f>
+        <v>814.34999999999945</v>
+      </c>
+      <c r="P85" s="33">
+        <f t="shared" si="57"/>
+        <v>813.58100000000002</v>
+      </c>
+      <c r="Q85" s="33">
+        <f t="shared" ref="Q85:S85" si="58">Q67-Q80</f>
+        <v>926.01500000000055</v>
+      </c>
+      <c r="R85" s="33">
+        <f t="shared" si="58"/>
+        <v>1068.2409999999998</v>
+      </c>
+      <c r="S85" s="33">
+        <f t="shared" si="58"/>
+        <v>867.39899999999943</v>
+      </c>
+      <c r="T85" s="33">
+        <f t="shared" ref="T85:U85" si="59">T67-T80</f>
+        <v>732.96799999999848</v>
+      </c>
+      <c r="U85" s="33">
+        <f t="shared" ref="U85:V85" si="60">U67-U80</f>
+        <v>746</v>
+      </c>
+      <c r="V85" s="33">
+        <f>V67-V80</f>
+        <v>720</v>
+      </c>
       <c r="W85" s="54"/>
     </row>
-    <row r="86" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="71"/>
-      <c r="F86" s="71"/>
-      <c r="H86" s="71"/>
-      <c r="J86" s="71"/>
-      <c r="L86" s="71"/>
-      <c r="S86" s="33">
-        <f t="shared" ref="S86:T86" si="41">+S60+S64</f>
-        <v>444.90699999999998</v>
-      </c>
-      <c r="T86" s="33">
-        <f t="shared" ref="T86:U86" si="42">+T60+T64</f>
-        <v>221.44899999999998</v>
-      </c>
-      <c r="U86" s="33">
-        <f t="shared" ref="U86:V86" si="43">+U60+U64</f>
-        <v>198</v>
-      </c>
-      <c r="V86" s="33">
-        <f>+V60+V64</f>
-        <v>238</v>
-      </c>
-      <c r="W86" s="54"/>
+    <row r="86" spans="2:23" s="53" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B86" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="D86" s="75"/>
+      <c r="F86" s="75"/>
+      <c r="H86" s="75"/>
+      <c r="J86" s="75"/>
+      <c r="L86" s="75"/>
+      <c r="O86" s="53">
+        <f t="shared" ref="O86" si="61">O85/O22</f>
+        <v>0.81396336740048425</v>
+      </c>
+      <c r="P86" s="53">
+        <f t="shared" ref="P86" si="62">P85/P22</f>
+        <v>0.81346060783004115</v>
+      </c>
+      <c r="Q86" s="53">
+        <f t="shared" ref="Q86" si="63">Q85/Q22</f>
+        <v>0.92541255642576747</v>
+      </c>
+      <c r="R86" s="53">
+        <f t="shared" ref="R86" si="64">R85/R22</f>
+        <v>1.067158900874513</v>
+      </c>
+      <c r="S86" s="53">
+        <f t="shared" ref="S86" si="65">S85/S22</f>
+        <v>0.86690486422738977</v>
+      </c>
+      <c r="T86" s="53">
+        <f t="shared" ref="T86" si="66">T85/T22</f>
+        <v>0.73245894103597842</v>
+      </c>
+      <c r="U86" s="53">
+        <f>U85/U22</f>
+        <v>0.74520933289779545</v>
+      </c>
+      <c r="V86" s="53">
+        <f>V85/V22</f>
+        <v>0.71885486420132727</v>
+      </c>
+      <c r="W86" s="87"/>
     </row>
     <row r="87" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B87" s="33" t="s">
-        <v>7</v>
-      </c>
       <c r="D87" s="71"/>
       <c r="F87" s="71"/>
       <c r="H87" s="71"/>
       <c r="J87" s="71"/>
       <c r="L87" s="71"/>
-      <c r="S87" s="33">
-        <f t="shared" ref="S87:T87" si="44">+S67+S72</f>
-        <v>773.40800000000002</v>
-      </c>
-      <c r="T87" s="33">
-        <f t="shared" ref="T87:U87" si="45">+T67+T72</f>
-        <v>730.61099999999999</v>
-      </c>
-      <c r="U87" s="33">
-        <f t="shared" ref="U87:V87" si="46">+U67+U72</f>
-        <v>956</v>
-      </c>
-      <c r="V87" s="33">
-        <f>+V67+V72</f>
-        <v>954</v>
-      </c>
       <c r="W87" s="54"/>
     </row>
     <row r="88" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B88" s="33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D88" s="71"/>
       <c r="F88" s="71"/>
@@ -4329,275 +4953,338 @@
       <c r="J88" s="71"/>
       <c r="L88" s="71"/>
       <c r="O88" s="33">
-        <f t="shared" ref="O88:U88" si="47">O86-O87</f>
-        <v>0</v>
+        <f t="shared" ref="O88:Q88" si="67">+O62+O66</f>
+        <v>95.917000000000002</v>
       </c>
       <c r="P88" s="33">
-        <f t="shared" si="47"/>
-        <v>0</v>
+        <f t="shared" si="67"/>
+        <v>155.92099999999999</v>
       </c>
       <c r="Q88" s="33">
-        <f t="shared" si="47"/>
-        <v>0</v>
+        <f t="shared" ref="Q88:S88" si="68">+Q62+Q66</f>
+        <v>90.816000000000003</v>
       </c>
       <c r="R88" s="33">
-        <f t="shared" si="47"/>
-        <v>0</v>
+        <f t="shared" si="68"/>
+        <v>89.983000000000004</v>
       </c>
       <c r="S88" s="33">
-        <f t="shared" si="47"/>
-        <v>-328.50100000000003</v>
+        <f t="shared" ref="S88:T88" si="69">+S62+S66</f>
+        <v>444.90699999999998</v>
       </c>
       <c r="T88" s="33">
-        <f t="shared" si="47"/>
-        <v>-509.16200000000003</v>
+        <f t="shared" ref="T88:U88" si="70">+T62+T66</f>
+        <v>221.44899999999998</v>
       </c>
       <c r="U88" s="33">
-        <f t="shared" si="47"/>
-        <v>-758</v>
+        <f t="shared" ref="U88:V88" si="71">+U62+U66</f>
+        <v>198</v>
       </c>
       <c r="V88" s="33">
-        <f>V86-V87</f>
-        <v>-716</v>
+        <f>+V62+V66</f>
+        <v>238</v>
       </c>
       <c r="W88" s="54"/>
     </row>
     <row r="89" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="33" t="s">
+        <v>7</v>
+      </c>
       <c r="D89" s="71"/>
       <c r="F89" s="71"/>
       <c r="H89" s="71"/>
       <c r="J89" s="71"/>
       <c r="L89" s="71"/>
+      <c r="O89" s="33">
+        <f t="shared" ref="O89:Q89" si="72">+O69+O74</f>
+        <v>451.18299999999999</v>
+      </c>
+      <c r="P89" s="33">
+        <f t="shared" si="72"/>
+        <v>561.61099999999999</v>
+      </c>
+      <c r="Q89" s="33">
+        <f t="shared" ref="Q89:S89" si="73">+Q69+Q74</f>
+        <v>630.95899999999995</v>
+      </c>
+      <c r="R89" s="33">
+        <f t="shared" si="73"/>
+        <v>692.85900000000004</v>
+      </c>
+      <c r="S89" s="33">
+        <f t="shared" ref="S89:T89" si="74">+S69+S74</f>
+        <v>773.40800000000002</v>
+      </c>
+      <c r="T89" s="33">
+        <f t="shared" ref="T89:U89" si="75">+T69+T74</f>
+        <v>730.61099999999999</v>
+      </c>
+      <c r="U89" s="33">
+        <f t="shared" ref="U89:V89" si="76">+U69+U74</f>
+        <v>956</v>
+      </c>
+      <c r="V89" s="33">
+        <f>+V69+V74</f>
+        <v>954</v>
+      </c>
       <c r="W89" s="54"/>
     </row>
-    <row r="90" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="D90" s="70"/>
-      <c r="F90" s="70"/>
-      <c r="H90" s="70"/>
-      <c r="J90" s="70"/>
-      <c r="L90" s="70"/>
-      <c r="T90" s="38">
-        <f>T61/S61-1</f>
-        <v>2.9125850340135928E-2</v>
-      </c>
-      <c r="U90" s="38">
-        <f>U61/T61-1</f>
-        <v>0.42614926478121928</v>
-      </c>
-      <c r="V90" s="38">
-        <f>V61/U61-1</f>
-        <v>-0.11471610660486675</v>
-      </c>
-      <c r="W90" s="84"/>
+    <row r="90" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B90" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D90" s="71"/>
+      <c r="F90" s="71"/>
+      <c r="H90" s="71"/>
+      <c r="J90" s="71"/>
+      <c r="L90" s="71"/>
+      <c r="O90" s="33">
+        <f t="shared" ref="O90:U90" si="77">O88-O89</f>
+        <v>-355.26599999999996</v>
+      </c>
+      <c r="P90" s="33">
+        <f t="shared" si="77"/>
+        <v>-405.69</v>
+      </c>
+      <c r="Q90" s="33">
+        <f t="shared" si="77"/>
+        <v>-540.14299999999992</v>
+      </c>
+      <c r="R90" s="33">
+        <f t="shared" si="77"/>
+        <v>-602.87599999999998</v>
+      </c>
+      <c r="S90" s="33">
+        <f t="shared" si="77"/>
+        <v>-328.50100000000003</v>
+      </c>
+      <c r="T90" s="33">
+        <f t="shared" si="77"/>
+        <v>-509.16200000000003</v>
+      </c>
+      <c r="U90" s="33">
+        <f t="shared" si="77"/>
+        <v>-758</v>
+      </c>
+      <c r="V90" s="33">
+        <f>V88-V89</f>
+        <v>-716</v>
+      </c>
+      <c r="W90" s="54"/>
     </row>
     <row r="91" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="33" t="s">
-        <v>105</v>
-      </c>
       <c r="D91" s="71"/>
       <c r="F91" s="71"/>
       <c r="H91" s="71"/>
       <c r="J91" s="71"/>
       <c r="L91" s="71"/>
-      <c r="O91" s="52" t="s">
+      <c r="W91" s="54"/>
+    </row>
+    <row r="92" spans="2:23" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B92" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D92" s="70"/>
+      <c r="F92" s="70"/>
+      <c r="H92" s="70"/>
+      <c r="J92" s="70"/>
+      <c r="L92" s="70"/>
+      <c r="O92" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="P91" s="52" t="s">
+      <c r="P92" s="38">
+        <f t="shared" ref="P92:T92" si="78">P63/O63-1</f>
+        <v>0.29695042546981298</v>
+      </c>
+      <c r="Q92" s="38">
+        <f t="shared" si="78"/>
+        <v>0.20897431181145976</v>
+      </c>
+      <c r="R92" s="38">
+        <f t="shared" si="78"/>
+        <v>0.20052444110329515</v>
+      </c>
+      <c r="S92" s="38">
+        <f t="shared" si="78"/>
+        <v>-0.12333145972766624</v>
+      </c>
+      <c r="T92" s="38">
+        <f>T63/S63-1</f>
+        <v>2.9125850340135928E-2</v>
+      </c>
+      <c r="U92" s="38">
+        <f>U63/T63-1</f>
+        <v>0.42614926478121928</v>
+      </c>
+      <c r="V92" s="38">
+        <f>V63/U63-1</f>
+        <v>-0.11471610660486675</v>
+      </c>
+      <c r="W92" s="84"/>
+    </row>
+    <row r="93" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B93" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D93" s="71"/>
+      <c r="F93" s="71"/>
+      <c r="H93" s="71"/>
+      <c r="J93" s="71"/>
+      <c r="L93" s="71"/>
+      <c r="O93" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="Q91" s="52" t="s">
+      <c r="P93" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="R91" s="52" t="s">
+      <c r="Q93" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="S91" s="52" t="s">
+      <c r="R93" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="T91" s="52" t="s">
+      <c r="S93" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="U91" s="52" t="s">
+      <c r="T93" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="V91" s="52" t="s">
+      <c r="U93" s="52" t="s">
         <v>74</v>
       </c>
-      <c r="W91" s="54"/>
-    </row>
-    <row r="92" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="33" t="s">
+      <c r="V93" s="52" t="s">
+        <v>74</v>
+      </c>
+      <c r="W93" s="54"/>
+    </row>
+    <row r="94" spans="2:23" s="33" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B94" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="D92" s="71"/>
-      <c r="F92" s="71"/>
-      <c r="H92" s="71"/>
-      <c r="J92" s="71"/>
-      <c r="L92" s="71"/>
-      <c r="O92" s="55"/>
-      <c r="P92" s="55"/>
-      <c r="Q92" s="55"/>
-      <c r="R92" s="55"/>
-      <c r="S92" s="55">
-        <f t="shared" ref="O92:V92" si="48">S61/S4</f>
+      <c r="D94" s="71"/>
+      <c r="F94" s="71"/>
+      <c r="H94" s="71"/>
+      <c r="J94" s="71"/>
+      <c r="L94" s="71"/>
+      <c r="O94" s="55">
+        <f t="shared" ref="O94:V94" si="79">O63/O4</f>
+        <v>0.1750673738567326</v>
+      </c>
+      <c r="P94" s="55">
+        <f t="shared" si="79"/>
+        <v>0.19012079023804238</v>
+      </c>
+      <c r="Q94" s="55">
+        <f t="shared" si="79"/>
+        <v>0.18439818839646949</v>
+      </c>
+      <c r="R94" s="55">
+        <f t="shared" si="79"/>
+        <v>0.1923879075063929</v>
+      </c>
+      <c r="S94" s="55">
+        <f t="shared" si="79"/>
         <v>0.15419363416301571</v>
       </c>
-      <c r="T92" s="55">
-        <f t="shared" si="48"/>
+      <c r="T94" s="55">
+        <f t="shared" si="79"/>
         <v>0.12603050136157493</v>
       </c>
-      <c r="U92" s="55">
-        <f t="shared" si="48"/>
+      <c r="U94" s="55">
+        <f t="shared" si="79"/>
         <v>0.18467793708538413</v>
       </c>
-      <c r="V92" s="55">
-        <f>V61/V4</f>
+      <c r="V94" s="55">
+        <f>V63/V4</f>
         <v>0.15332129239414008</v>
       </c>
-      <c r="W92" s="54"/>
-    </row>
-    <row r="94" spans="2:23" s="40" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B94" s="40" t="s">
+      <c r="W94" s="54"/>
+    </row>
+    <row r="96" spans="2:23" s="40" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B96" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D94" s="68"/>
-      <c r="F94" s="68"/>
-      <c r="H94" s="68"/>
-      <c r="J94" s="68"/>
-      <c r="L94" s="68"/>
-      <c r="S94" s="40">
+      <c r="D96" s="68"/>
+      <c r="F96" s="68"/>
+      <c r="H96" s="68"/>
+      <c r="J96" s="68"/>
+      <c r="L96" s="68"/>
+      <c r="S96" s="40">
         <v>2.0379999999999998</v>
       </c>
-      <c r="T94" s="40">
+      <c r="T96" s="40">
         <v>4.5180999999999996</v>
       </c>
-      <c r="U94" s="40">
+      <c r="U96" s="40">
         <v>5.0332999999999997</v>
       </c>
-      <c r="V94" s="40">
+      <c r="V96" s="40">
         <v>4.6698000000000004</v>
       </c>
-      <c r="W94" s="81"/>
-    </row>
-    <row r="95" spans="2:23" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B95" s="49" t="s">
+      <c r="W96" s="81"/>
+    </row>
+    <row r="97" spans="2:23" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B97" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="D95" s="73"/>
-      <c r="F95" s="73"/>
-      <c r="H95" s="73"/>
-      <c r="J95" s="73"/>
-      <c r="L95" s="73"/>
-      <c r="S95" s="49">
-        <f t="shared" ref="S95" si="49">S94*S22</f>
+      <c r="D97" s="73"/>
+      <c r="F97" s="73"/>
+      <c r="H97" s="73"/>
+      <c r="J97" s="73"/>
+      <c r="L97" s="73"/>
+      <c r="S97" s="49">
+        <f t="shared" ref="S97" si="80">S96*S22</f>
         <v>2039.16166</v>
       </c>
-      <c r="T95" s="49">
-        <f t="shared" ref="T95" si="50">T94*T22</f>
+      <c r="T97" s="49">
+        <f t="shared" ref="T97" si="81">T96*T22</f>
         <v>4521.2400794999994</v>
       </c>
-      <c r="U95" s="49">
-        <f t="shared" ref="U95" si="51">U94*U22</f>
+      <c r="U97" s="49">
+        <f t="shared" ref="U97" si="82">U96*U22</f>
         <v>5038.6403313000001</v>
       </c>
-      <c r="V95" s="49">
-        <f>V94*V22</f>
+      <c r="V97" s="49">
+        <f>V96*V22</f>
         <v>4677.2389914000005</v>
       </c>
-      <c r="W95" s="54"/>
-    </row>
-    <row r="96" spans="2:23" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="49" t="s">
+      <c r="W97" s="54"/>
+    </row>
+    <row r="98" spans="2:23" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B98" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D96" s="73"/>
-      <c r="F96" s="73"/>
-      <c r="H96" s="73"/>
-      <c r="J96" s="73"/>
-      <c r="L96" s="73"/>
-      <c r="S96" s="49">
-        <f t="shared" ref="S96" si="52">S95-S88</f>
+      <c r="D98" s="73"/>
+      <c r="F98" s="73"/>
+      <c r="H98" s="73"/>
+      <c r="J98" s="73"/>
+      <c r="L98" s="73"/>
+      <c r="S98" s="49">
+        <f t="shared" ref="S98" si="83">S97-S90</f>
         <v>2367.66266</v>
       </c>
-      <c r="T96" s="49">
-        <f t="shared" ref="T96" si="53">T95-T88</f>
+      <c r="T98" s="49">
+        <f t="shared" ref="T98" si="84">T97-T90</f>
         <v>5030.4020794999997</v>
       </c>
-      <c r="U96" s="49">
-        <f t="shared" ref="U96" si="54">U95-U88</f>
+      <c r="U98" s="49">
+        <f t="shared" ref="U98" si="85">U97-U90</f>
         <v>5796.6403313000001</v>
       </c>
-      <c r="V96" s="49">
-        <f>V95-V88</f>
+      <c r="V98" s="49">
+        <f>V97-V90</f>
         <v>5393.2389914000005</v>
       </c>
-      <c r="W96" s="54"/>
-    </row>
-    <row r="98" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B98" s="39" t="s">
+      <c r="W98" s="54"/>
+    </row>
+    <row r="100" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="B100" s="39" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="99" spans="2:23" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B99" s="60" t="s">
-        <v>31</v>
-      </c>
-      <c r="D99" s="74"/>
-      <c r="F99" s="74"/>
-      <c r="H99" s="74"/>
-      <c r="J99" s="74"/>
-      <c r="L99" s="74"/>
-      <c r="S99" s="63">
-        <f t="shared" ref="S99:V99" si="55">S94/S84</f>
-        <v>2.3508923344389392</v>
-      </c>
-      <c r="T99" s="63">
-        <f t="shared" si="55"/>
-        <v>6.1684003660460069</v>
-      </c>
-      <c r="U99" s="63">
-        <f t="shared" si="55"/>
-        <v>6.7542095593833773</v>
-      </c>
-      <c r="V99" s="63">
-        <f>V94/V84</f>
-        <v>6.4961652658333344</v>
-      </c>
-      <c r="W99" s="86"/>
-    </row>
-    <row r="100" spans="2:23" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B100" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="D100" s="74"/>
-      <c r="F100" s="74"/>
-      <c r="H100" s="74"/>
-      <c r="J100" s="74"/>
-      <c r="L100" s="74"/>
-      <c r="S100" s="63">
-        <f t="shared" ref="S100:V100" si="56">S95/S4</f>
-        <v>0.53473766496817654</v>
-      </c>
-      <c r="T100" s="63">
-        <f t="shared" si="56"/>
-        <v>0.94164546556491024</v>
-      </c>
-      <c r="U100" s="63">
-        <f t="shared" si="56"/>
-        <v>1.0782453095013911</v>
-      </c>
-      <c r="V100" s="63">
-        <f>V95/V4</f>
-        <v>0.93863917146297426</v>
-      </c>
-      <c r="W100" s="86"/>
     </row>
     <row r="101" spans="2:23" s="60" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B101" s="60" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D101" s="74"/>
       <c r="F101" s="74"/>
@@ -4605,80 +5292,107 @@
       <c r="J101" s="74"/>
       <c r="L101" s="74"/>
       <c r="S101" s="63">
-        <f t="shared" ref="S101:V101" si="57">S94/S21</f>
+        <f t="shared" ref="S101:V101" si="86">S96/S86</f>
+        <v>2.3508923344389392</v>
+      </c>
+      <c r="T101" s="63">
+        <f t="shared" si="86"/>
+        <v>6.1684003660460069</v>
+      </c>
+      <c r="U101" s="63">
+        <f t="shared" si="86"/>
+        <v>6.7542095593833773</v>
+      </c>
+      <c r="V101" s="63">
+        <f>V96/V86</f>
+        <v>6.4961652658333344</v>
+      </c>
+      <c r="W101" s="86"/>
+    </row>
+    <row r="102" spans="2:23" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B102" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="D102" s="74"/>
+      <c r="F102" s="74"/>
+      <c r="H102" s="74"/>
+      <c r="J102" s="74"/>
+      <c r="L102" s="74"/>
+      <c r="S102" s="63">
+        <f t="shared" ref="S102:V102" si="87">S97/S4</f>
+        <v>0.53473766496817654</v>
+      </c>
+      <c r="T102" s="63">
+        <f t="shared" si="87"/>
+        <v>0.94164546556491024</v>
+      </c>
+      <c r="U102" s="63">
+        <f t="shared" si="87"/>
+        <v>1.0782453095013911</v>
+      </c>
+      <c r="V102" s="63">
+        <f>V97/V4</f>
+        <v>0.93863917146297426</v>
+      </c>
+      <c r="W102" s="86"/>
+    </row>
+    <row r="103" spans="2:23" s="60" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B103" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="D103" s="74"/>
+      <c r="F103" s="74"/>
+      <c r="H103" s="74"/>
+      <c r="J103" s="74"/>
+      <c r="L103" s="74"/>
+      <c r="S103" s="63">
+        <f t="shared" ref="S103:V103" si="88">S96/S21</f>
         <v>10.008941364720664</v>
       </c>
-      <c r="T101" s="63">
-        <f t="shared" si="57"/>
+      <c r="T103" s="63">
+        <f t="shared" si="88"/>
         <v>11.015271163254162</v>
       </c>
-      <c r="U101" s="63">
-        <f t="shared" si="57"/>
+      <c r="U103" s="63">
+        <f t="shared" si="88"/>
         <v>11.556514521330275</v>
       </c>
-      <c r="V101" s="63">
-        <f>V94/V21</f>
+      <c r="V103" s="63">
+        <f>V96/V21</f>
         <v>12.117199459585493</v>
       </c>
-      <c r="W101" s="86"/>
-    </row>
-    <row r="102" spans="2:23" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B102" s="50" t="s">
+      <c r="W103" s="86"/>
+    </row>
+    <row r="104" spans="2:23" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B104" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="D102" s="76"/>
-      <c r="F102" s="76"/>
-      <c r="H102" s="76"/>
-      <c r="J102" s="76"/>
-      <c r="L102" s="76"/>
-      <c r="S102" s="62">
-        <f t="shared" ref="S102:V102" si="58">S96/S4</f>
+      <c r="D104" s="76"/>
+      <c r="F104" s="76"/>
+      <c r="H104" s="76"/>
+      <c r="J104" s="76"/>
+      <c r="L104" s="76"/>
+      <c r="S104" s="62">
+        <f t="shared" ref="S104:V104" si="89">S98/S4</f>
         <v>0.62088181975760648</v>
       </c>
-      <c r="T102" s="62">
-        <f t="shared" si="58"/>
+      <c r="T104" s="62">
+        <f t="shared" si="89"/>
         <v>1.0476894004384114</v>
       </c>
-      <c r="U102" s="62">
-        <f t="shared" si="58"/>
+      <c r="U104" s="62">
+        <f t="shared" si="89"/>
         <v>1.2404537409158998</v>
       </c>
-      <c r="V102" s="62">
-        <f>V96/V4</f>
+      <c r="V104" s="62">
+        <f>V98/V4</f>
         <v>1.0823277125025086</v>
       </c>
-      <c r="W102" s="88"/>
-    </row>
-    <row r="103" spans="2:23" s="50" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B103" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="D103" s="76"/>
-      <c r="F103" s="76"/>
-      <c r="H103" s="76"/>
-      <c r="J103" s="76"/>
-      <c r="L103" s="76"/>
-      <c r="S103" s="62">
-        <f t="shared" ref="S103:V103" si="59">S96/S20</f>
-        <v>11.621342829375557</v>
-      </c>
-      <c r="T103" s="62">
-        <f t="shared" si="59"/>
-        <v>12.255762134183771</v>
-      </c>
-      <c r="U103" s="62">
-        <f t="shared" si="59"/>
-        <v>13.295046631422018</v>
-      </c>
-      <c r="V103" s="62">
-        <f>V96/V20</f>
-        <v>13.97212173937824</v>
-      </c>
-      <c r="W103" s="88"/>
+      <c r="W104" s="88"/>
     </row>
     <row r="105" spans="2:23" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B105" s="50" t="s">
-        <v>130</v>
+        <v>35</v>
       </c>
       <c r="D105" s="76"/>
       <c r="F105" s="76"/>
@@ -4686,34 +5400,63 @@
       <c r="J105" s="76"/>
       <c r="L105" s="76"/>
       <c r="S105" s="62">
-        <f t="shared" ref="S105:V105" si="60">S87/S80</f>
+        <f t="shared" ref="S105:V105" si="90">S98/S20</f>
+        <v>11.621342829375557</v>
+      </c>
+      <c r="T105" s="62">
+        <f t="shared" si="90"/>
+        <v>12.255762134183771</v>
+      </c>
+      <c r="U105" s="62">
+        <f t="shared" si="90"/>
+        <v>13.295046631422018</v>
+      </c>
+      <c r="V105" s="62">
+        <f>V98/V20</f>
+        <v>13.97212173937824</v>
+      </c>
+      <c r="W105" s="88"/>
+    </row>
+    <row r="107" spans="2:23" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B107" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="D107" s="76"/>
+      <c r="F107" s="76"/>
+      <c r="H107" s="76"/>
+      <c r="J107" s="76"/>
+      <c r="L107" s="76"/>
+      <c r="S107" s="62">
+        <f t="shared" ref="S107:V107" si="91">S89/S82</f>
         <v>0.89164041000738992</v>
       </c>
-      <c r="T105" s="62">
-        <f t="shared" si="60"/>
+      <c r="T107" s="62">
+        <f t="shared" si="91"/>
         <v>0.99678430709116905</v>
       </c>
-      <c r="U105" s="62">
-        <f t="shared" si="60"/>
+      <c r="U107" s="62">
+        <f t="shared" si="91"/>
         <v>1.2815013404825737</v>
       </c>
-      <c r="V105" s="62">
-        <f>V87/V80</f>
+      <c r="V107" s="62">
+        <f>V89/V82</f>
         <v>1.325</v>
       </c>
-      <c r="W105" s="88"/>
+      <c r="W107" s="88"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="V1" r:id="rId1" location="page=1" xr:uid="{E121E959-3971-4F0C-9D31-6597A2936EC2}"/>
     <hyperlink ref="T1" r:id="rId2" xr:uid="{7837FB7C-00FB-40DB-8535-E935902869EF}"/>
+    <hyperlink ref="R1" r:id="rId3" xr:uid="{234D5C46-CFB8-4EFF-B019-5A96317C7ED5}"/>
+    <hyperlink ref="P1" r:id="rId4" xr:uid="{3F26C874-BA3D-4574-85A7-9E2A3E0932A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="125" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
+  <pageSetup paperSize="125" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId5"/>
   <ignoredErrors>
     <ignoredError sqref="S7" formula="1"/>
   </ignoredErrors>
-  <drawing r:id="rId4"/>
-  <legacyDrawing r:id="rId5"/>
+  <drawing r:id="rId6"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
£BME Wilko stores update
</commit_message>
<xml_diff>
--- a/£BME.xlsx
+++ b/£BME.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\My Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1CCDC7-4F4F-4BC1-B675-8A84E417E3B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E720BB-7135-493C-88A8-F0BC28C14474}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{0B0D3E06-E58D-4F1F-A8B8-3BC216B2A3D5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B0D3E06-E58D-4F1F-A8B8-3BC216B2A3D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -69,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="154">
   <si>
     <t>£BME</t>
   </si>
@@ -528,6 +519,9 @@
   </si>
   <si>
     <t>Upside</t>
+  </si>
+  <si>
+    <t>B&amp;M confirm entered an agreement to acquire up to 51 properties from Wilko Ltd. For a max consideration of £13m</t>
   </si>
 </sst>
 </file>
@@ -804,7 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -976,6 +970,7 @@
     <xf numFmtId="2" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1498,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF562411-448F-49B1-B6D6-24D041947C33}">
   <dimension ref="B2:X41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1518,35 +1513,35 @@
       </c>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="T4" s="115" t="s">
+      <c r="T4" s="116" t="s">
         <v>125</v>
       </c>
-      <c r="U4" s="117"/>
-      <c r="W4" s="115" t="s">
+      <c r="U4" s="118"/>
+      <c r="W4" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="X4" s="117"/>
+      <c r="X4" s="118"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="116"/>
-      <c r="D5" s="117"/>
-      <c r="F5" s="115" t="s">
+      <c r="C5" s="117"/>
+      <c r="D5" s="118"/>
+      <c r="F5" s="116" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="116"/>
-      <c r="H5" s="116"/>
-      <c r="I5" s="116"/>
-      <c r="J5" s="116"/>
-      <c r="K5" s="116"/>
-      <c r="L5" s="116"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="116"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="116"/>
-      <c r="Q5" s="117"/>
+      <c r="G5" s="117"/>
+      <c r="H5" s="117"/>
+      <c r="I5" s="117"/>
+      <c r="J5" s="117"/>
+      <c r="K5" s="117"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="117"/>
+      <c r="N5" s="117"/>
+      <c r="O5" s="117"/>
+      <c r="P5" s="117"/>
+      <c r="Q5" s="118"/>
       <c r="T5" s="41" t="s">
         <v>25</v>
       </c>
@@ -1560,7 +1555,7 @@
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="30">
         <v>5.7348999999999997</v>
       </c>
       <c r="D6" s="16"/>
@@ -1625,8 +1620,12 @@
         <v>5744.0356956999995</v>
       </c>
       <c r="D8" s="16"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="5"/>
+      <c r="F8" s="44">
+        <v>45170</v>
+      </c>
+      <c r="G8" s="111" t="s">
+        <v>153</v>
+      </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -1786,11 +1785,11 @@
       <c r="Q14" s="6"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B15" s="115" t="s">
+      <c r="B15" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="116"/>
-      <c r="D15" s="117"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="118"/>
       <c r="F15" s="12"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -1808,10 +1807,10 @@
       <c r="B16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="122" t="s">
+      <c r="C16" s="123" t="s">
         <v>21</v>
       </c>
-      <c r="D16" s="119"/>
+      <c r="D16" s="120"/>
       <c r="F16" s="12"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -1829,10 +1828,10 @@
       <c r="B17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="122" t="s">
+      <c r="C17" s="123" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="119"/>
+      <c r="D17" s="120"/>
       <c r="F17" s="12"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -1850,8 +1849,8 @@
       <c r="B18" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="122"/>
-      <c r="D18" s="119"/>
+      <c r="C18" s="123"/>
+      <c r="D18" s="120"/>
       <c r="F18" s="44">
         <v>43891</v>
       </c>
@@ -1873,10 +1872,10 @@
       <c r="B19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="113" t="s">
+      <c r="C19" s="114" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="114"/>
+      <c r="D19" s="115"/>
       <c r="F19" s="12"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1919,11 +1918,11 @@
       <c r="Q21" s="6"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B22" s="115" t="s">
+      <c r="B22" s="116" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="116"/>
-      <c r="D22" s="117"/>
+      <c r="C22" s="117"/>
+      <c r="D22" s="118"/>
       <c r="F22" s="12"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
@@ -1941,10 +1940,10 @@
       <c r="B23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="122" t="s">
+      <c r="C23" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="119"/>
+      <c r="D23" s="120"/>
       <c r="F23" s="44">
         <v>42948</v>
       </c>
@@ -1966,10 +1965,10 @@
       <c r="B24" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="122">
+      <c r="C24" s="123">
         <v>1978</v>
       </c>
-      <c r="D24" s="119"/>
+      <c r="D24" s="120"/>
       <c r="F24" s="12"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
@@ -1987,10 +1986,10 @@
       <c r="B25" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="122">
+      <c r="C25" s="123">
         <v>2014</v>
       </c>
-      <c r="D25" s="119"/>
+      <c r="D25" s="120"/>
       <c r="F25" s="12"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
@@ -2006,8 +2005,8 @@
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="12"/>
-      <c r="C26" s="122"/>
-      <c r="D26" s="119"/>
+      <c r="C26" s="123"/>
+      <c r="D26" s="120"/>
       <c r="F26" s="12"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -2025,11 +2024,11 @@
       <c r="B27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C27" s="118">
+      <c r="C27" s="119">
         <f>+'Financial Model'!V34</f>
         <v>1140</v>
       </c>
-      <c r="D27" s="119"/>
+      <c r="D27" s="120"/>
       <c r="F27" s="12"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
@@ -2047,11 +2046,11 @@
       <c r="B28" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="118">
+      <c r="C28" s="119">
         <f>+'Financial Model'!V67</f>
         <v>764</v>
       </c>
-      <c r="D28" s="119"/>
+      <c r="D28" s="120"/>
       <c r="F28" s="12"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
@@ -2069,11 +2068,11 @@
       <c r="B29" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="118">
+      <c r="C29" s="119">
         <f>'Financial Model'!V46</f>
         <v>39484</v>
       </c>
-      <c r="D29" s="119"/>
+      <c r="D29" s="120"/>
       <c r="F29" s="12"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -2131,10 +2130,10 @@
       <c r="B32" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="120" t="s">
+      <c r="C32" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="121"/>
+      <c r="D32" s="122"/>
       <c r="F32" s="12"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
@@ -2177,11 +2176,11 @@
       <c r="Q34" s="6"/>
     </row>
     <row r="35" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B35" s="115" t="s">
+      <c r="B35" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="116"/>
-      <c r="D35" s="117"/>
+      <c r="C35" s="117"/>
+      <c r="D35" s="118"/>
       <c r="F35" s="12"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
@@ -2199,11 +2198,11 @@
       <c r="B36" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C36" s="111">
+      <c r="C36" s="112">
         <f>C6/'Financial Model'!V90</f>
         <v>7.9778273551388885</v>
       </c>
-      <c r="D36" s="112"/>
+      <c r="D36" s="113"/>
       <c r="F36" s="12"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
@@ -2221,11 +2220,11 @@
       <c r="B37" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="111">
+      <c r="C37" s="112">
         <f>C8/'Financial Model'!V4</f>
         <v>1.152726408930363</v>
       </c>
-      <c r="D37" s="112"/>
+      <c r="D37" s="113"/>
       <c r="F37" s="12"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
@@ -2243,11 +2242,11 @@
       <c r="B38" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C38" s="111">
+      <c r="C38" s="112">
         <f>C12/'Financial Model'!V4</f>
         <v>1.2964149499698976</v>
       </c>
-      <c r="D38" s="112"/>
+      <c r="D38" s="113"/>
       <c r="F38" s="12"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
@@ -2265,11 +2264,11 @@
       <c r="B39" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="111">
+      <c r="C39" s="112">
         <f>C6/'Financial Model'!V21</f>
         <v>14.880921491450774</v>
       </c>
-      <c r="D39" s="112"/>
+      <c r="D39" s="113"/>
       <c r="F39" s="12"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
@@ -2287,11 +2286,11 @@
       <c r="B40" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="111">
+      <c r="C40" s="112">
         <f>C12/'Financial Model'!V16</f>
         <v>18.563320964655169</v>
       </c>
-      <c r="D40" s="112"/>
+      <c r="D40" s="113"/>
       <c r="F40" s="12"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
@@ -2309,8 +2308,8 @@
       <c r="B41" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="113"/>
-      <c r="D41" s="114"/>
+      <c r="C41" s="114"/>
+      <c r="D41" s="115"/>
       <c r="F41" s="13"/>
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
@@ -2355,10 +2354,11 @@
   <hyperlinks>
     <hyperlink ref="C32:D32" r:id="rId1" display="Link" xr:uid="{9BE3B3D4-9498-4B97-998C-C0C12FA77148}"/>
     <hyperlink ref="G18" r:id="rId2" xr:uid="{87BBEC1A-B702-4F90-99BE-E634A1207125}"/>
+    <hyperlink ref="G8" r:id="rId3" xr:uid="{476FE842-C08E-4E0C-AE6F-086836C6516E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="125" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup paperSize="125" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -2366,11 +2366,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E38EA70-0C15-460C-B41E-267C906FFAC5}">
   <dimension ref="B1:DR111"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AH28" sqref="AH28"/>
+      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2613,11 +2613,26 @@
         <v>41</v>
       </c>
       <c r="C4" s="19"/>
-      <c r="D4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="J4" s="51"/>
-      <c r="L4" s="51"/>
+      <c r="D4" s="55">
+        <f>R4-C4</f>
+        <v>3486.2950000000001</v>
+      </c>
+      <c r="F4" s="55">
+        <f>S4-E4</f>
+        <v>3813.3870000000002</v>
+      </c>
+      <c r="H4" s="55">
+        <f>T4-G4</f>
+        <v>4801.4250000000002</v>
+      </c>
+      <c r="J4" s="55">
+        <f>U4-I4</f>
+        <v>4673</v>
+      </c>
+      <c r="L4" s="55">
+        <f>V4-K4</f>
+        <v>4983</v>
+      </c>
       <c r="O4" s="22">
         <v>2035.2850000000001</v>
       </c>
@@ -4794,7 +4809,10 @@
         <f>+V35+V38+V40</f>
         <v>1140</v>
       </c>
-      <c r="W34" s="69"/>
+      <c r="W34" s="69">
+        <f>V34+51</f>
+        <v>1191</v>
+      </c>
       <c r="X34" s="90"/>
       <c r="Y34" s="90"/>
       <c r="Z34" s="90"/>

</xml_diff>